<commit_message>
update wbs and astah
</commit_message>
<xml_diff>
--- a/_project_docs/SSE19_SPP_WBS.xlsx
+++ b/_project_docs/SSE19_SPP_WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workplace\smartse19\_project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9EE711-0158-4762-8D29-3A92EF72C7CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED3B7D-B2F6-4762-A613-9DEF7C856660}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{D3C1DD7E-20E6-4452-8E15-DB8203761C57}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="253">
   <si>
     <t>No</t>
   </si>
@@ -764,6 +764,39 @@
   </si>
   <si>
     <t>Iter-pre</t>
+  </si>
+  <si>
+    <t>プロトタイプ事前検証</t>
+  </si>
+  <si>
+    <t>Validation for Prototyping</t>
+  </si>
+  <si>
+    <t>VALID</t>
+  </si>
+  <si>
+    <t>keystrokes</t>
+  </si>
+  <si>
+    <t>PC Monitoring (Key Strokeを監視）</t>
+  </si>
+  <si>
+    <t>ActiveWindows</t>
+  </si>
+  <si>
+    <t>PC Monitoring (Active Windowを監視）</t>
+  </si>
+  <si>
+    <t>検証用プロトタイプ</t>
+  </si>
+  <si>
+    <t>activewindow</t>
+  </si>
+  <si>
+    <t>pcactiveinfo</t>
+  </si>
+  <si>
+    <t>PC Monitoringデータを加工</t>
   </si>
 </sst>
 </file>
@@ -935,7 +968,147 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1277,13 +1450,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:O111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomRight" activeCell="M54" sqref="M54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1532,7 +1705,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <f t="shared" ref="A9:A79" si="3">ROW()-4</f>
+        <f t="shared" ref="A9:A84" si="3">ROW()-4</f>
         <v>5</v>
       </c>
       <c r="B9" s="1">
@@ -2171,7 +2344,7 @@
         <v>13</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>47</v>
@@ -2216,7 +2389,9 @@
       <c r="J24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="1"/>
+      <c r="K24" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="L24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2260,7 +2435,9 @@
       <c r="J25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="K25" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="L25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2286,7 +2463,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f t="shared" ref="E26:E105" si="13">TEXT(B26,"00")&amp;IF(C26="","","-"&amp;TEXT(C26,"00"))&amp;IF(D26="","","-"&amp;TEXT(D26,"00"))</f>
+        <f t="shared" ref="E26:E110" si="13">TEXT(B26,"00")&amp;IF(C26="","","-"&amp;TEXT(C26,"00"))&amp;IF(D26="","","-"&amp;TEXT(D26,"00"))</f>
         <v>03-01-03</v>
       </c>
       <c r="F26" s="1" t="s">
@@ -2304,7 +2481,9 @@
       <c r="J26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="K26" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="L26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2348,7 +2527,9 @@
       <c r="J27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="K27" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="L27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2392,7 +2573,9 @@
       <c r="J28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="L28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2644,7 +2827,7 @@
         <v>13</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>136</v>
+        <v>207</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>100</v>
@@ -2683,19 +2866,21 @@
       <c r="H35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I35" s="4" t="s">
-        <v>23</v>
+      <c r="I35" s="4">
+        <v>4</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K35" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="L35" s="1" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="M35" s="1" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>SSE19_RD_UXD</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -3337,14 +3522,12 @@
         <v>05</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>173</v>
+        <v>242</v>
       </c>
       <c r="G50" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>165</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="H50" s="6"/>
       <c r="I50" s="7"/>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -3366,31 +3549,25 @@
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="str">
-        <f t="shared" ref="E51:E58" si="18">TEXT(B51,"00")&amp;IF(C51="","","-"&amp;TEXT(C51,"00"))&amp;IF(D51="","","-"&amp;TEXT(D51,"00"))</f>
+        <f t="shared" ref="E51:E54" si="18">TEXT(B51,"00")&amp;IF(C51="","","-"&amp;TEXT(C51,"00"))&amp;IF(D51="","","-"&amp;TEXT(D51,"00"))</f>
         <v>05-01</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>174</v>
-      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="15" t="s">
-        <v>175</v>
+        <v>249</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I51" s="4">
-        <v>8</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J51" s="1"/>
       <c r="K51" s="1"/>
-      <c r="L51" s="1" t="s">
-        <v>188</v>
-      </c>
+      <c r="L51" s="1"/>
       <c r="M51" s="1" t="str">
-        <f t="shared" ref="M51:M58" si="19">IF(I51="↑","",IF(I51="-","",System_Code&amp;"_"&amp;H51&amp;IF(L51="-","","_"&amp;L51)))</f>
-        <v>SSE19_CD_CUSTD</v>
+        <f>IF(I51="↑","",IF(I51="-","",System_Code&amp;"_"&amp;H51&amp;IF(L51="-","","_"&amp;L51)))</f>
+        <v/>
       </c>
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
@@ -3404,39 +3581,37 @@
         <v>5</v>
       </c>
       <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D52" s="1"/>
       <c r="E52" s="1" t="str">
         <f t="shared" si="18"/>
-        <v>05-01-01</v>
+        <v>05-02</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>94</v>
+        <v>245</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>246</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>23</v>
+        <v>244</v>
+      </c>
+      <c r="I52" s="4">
+        <v>12</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>23</v>
+        <v>245</v>
       </c>
       <c r="M52" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f>IF(I52="↑","",IF(I52="-","",System_Code&amp;"_"&amp;H52&amp;IF(L52="-","","_"&amp;L52)))</f>
+        <v>SSE19_VALID_keystrokes</v>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -3450,39 +3625,37 @@
         <v>5</v>
       </c>
       <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D53" s="1"/>
       <c r="E53" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>05-01-02</v>
+        <f t="shared" ref="E53" si="19">TEXT(B53,"00")&amp;IF(C53="","","-"&amp;TEXT(C53,"00"))&amp;IF(D53="","","-"&amp;TEXT(D53,"00"))</f>
+        <v>05-03</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>95</v>
+        <v>247</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>248</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>23</v>
+        <v>244</v>
+      </c>
+      <c r="I53" s="4">
+        <v>12</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>132</v>
+        <v>207</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>23</v>
+        <v>250</v>
       </c>
       <c r="M53" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v/>
+        <f>IF(I53="↑","",IF(I53="-","",System_Code&amp;"_"&amp;H53&amp;IF(L53="-","","_"&amp;L53)))</f>
+        <v>SSE19_VALID_activewindow</v>
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -3496,35 +3669,37 @@
         <v>5</v>
       </c>
       <c r="C54" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="str">
         <f t="shared" si="18"/>
-        <v>05-02</v>
+        <v>05-04</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>172</v>
+        <v>251</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>165</v>
+        <v>244</v>
       </c>
       <c r="I54" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K54" s="1"/>
+      <c r="K54" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="L54" s="1" t="s">
-        <v>189</v>
+        <v>251</v>
       </c>
       <c r="M54" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>SSE19_CD_CUST_IV</v>
+        <f>IF(I54="↑","",IF(I54="-","",System_Code&amp;"_"&amp;H54&amp;IF(L54="-","","_"&amp;L54)))</f>
+        <v>SSE19_VALID_pcactiveinfo</v>
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -3535,43 +3710,30 @@
         <v>51</v>
       </c>
       <c r="B55" s="1">
-        <v>5</v>
-      </c>
-      <c r="C55" s="1">
-        <v>2</v>
-      </c>
-      <c r="D55" s="1">
-        <v>1</v>
-      </c>
-      <c r="E55" s="1" t="str">
-        <f t="shared" ref="E55:E56" si="20">TEXT(B55,"00")&amp;IF(C55="","","-"&amp;TEXT(C55,"00"))&amp;IF(D55="","","-"&amp;TEXT(D55,"00"))</f>
-        <v>05-02-01</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="H55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="6" t="str">
+        <f>TEXT(B55,"00")&amp;IF(C55="","","-"&amp;TEXT(C55,"00"))&amp;IF(D55="","",TEXT(D55,"00"))</f>
+        <v>06</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G55" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H55" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I55" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M55" s="1" t="str">
-        <f t="shared" ref="M55:M56" si="21">IF(I55="↑","",IF(I55="-","",System_Code&amp;"_"&amp;H55&amp;IF(L55="-","","_"&amp;L55)))</f>
-        <v/>
-      </c>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
@@ -3579,85 +3741,85 @@
         <v>52</v>
       </c>
       <c r="B56" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C56" s="1">
-        <v>2</v>
-      </c>
-      <c r="D56" s="1">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D56" s="1"/>
       <c r="E56" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v>05-02-02</v>
+        <f t="shared" ref="E56:E63" si="20">TEXT(B56,"00")&amp;IF(C56="","","-"&amp;TEXT(C56,"00"))&amp;IF(D56="","","-"&amp;TEXT(D56,"00"))</f>
+        <v>06-01</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G56" s="16" t="s">
-        <v>183</v>
+        <v>174</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I56" s="4" t="s">
-        <v>23</v>
+      <c r="I56" s="4">
+        <v>8</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K56" s="1"/>
       <c r="L56" s="1" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
       <c r="M56" s="1" t="str">
+        <f t="shared" ref="M56:M63" si="21">IF(I56="↑","",IF(I56="-","",System_Code&amp;"_"&amp;H56&amp;IF(L56="-","","_"&amp;L56)))</f>
+        <v>SSE19_CD_CUSTD</v>
+      </c>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A57" s="1">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="B57" s="1">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>06-01-01</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G57" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M57" s="1" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A57" s="1">
-        <f t="shared" si="3"/>
-        <v>53</v>
-      </c>
-      <c r="B57" s="1">
-        <v>5</v>
-      </c>
-      <c r="C57" s="1">
-        <v>2</v>
-      </c>
-      <c r="D57" s="1">
-        <v>3</v>
-      </c>
-      <c r="E57" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>05-02-03</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M57" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
@@ -3667,23 +3829,23 @@
         <v>54</v>
       </c>
       <c r="B58" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C58" s="1">
+        <v>1</v>
+      </c>
+      <c r="D58" s="1">
         <v>2</v>
       </c>
-      <c r="D58" s="1">
-        <v>4</v>
-      </c>
       <c r="E58" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>05-02-04</v>
+        <f t="shared" si="20"/>
+        <v>06-01-02</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>179</v>
+        <v>92</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>185</v>
+        <v>95</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>165</v>
@@ -3694,12 +3856,14 @@
       <c r="J58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K58" s="1"/>
+      <c r="K58" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L58" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M58" s="1" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="N58" s="1"/>
@@ -3711,40 +3875,38 @@
         <v>55</v>
       </c>
       <c r="B59" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C59" s="1">
         <v>2</v>
       </c>
-      <c r="D59" s="1">
-        <v>5</v>
-      </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="1" t="str">
-        <f t="shared" ref="E59:E60" si="22">TEXT(B59,"00")&amp;IF(C59="","","-"&amp;TEXT(C59,"00"))&amp;IF(D59="","","-"&amp;TEXT(D59,"00"))</f>
-        <v>05-02-05</v>
+        <f t="shared" si="20"/>
+        <v>06-02</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G59" s="16" t="s">
-        <v>186</v>
+        <v>172</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="I59" s="4" t="s">
-        <v>23</v>
+      <c r="I59" s="4">
+        <v>10</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K59" s="1"/>
       <c r="L59" s="1" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="M59" s="1" t="str">
-        <f t="shared" ref="M59:M60" si="23">IF(I59="↑","",IF(I59="-","",System_Code&amp;"_"&amp;H59&amp;IF(L59="-","","_"&amp;L59)))</f>
-        <v/>
+        <f t="shared" si="21"/>
+        <v>SSE19_CD_CUST_IV</v>
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -3755,23 +3917,23 @@
         <v>56</v>
       </c>
       <c r="B60" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1">
         <v>2</v>
       </c>
       <c r="D60" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f t="shared" si="22"/>
-        <v>05-02-06</v>
+        <f t="shared" ref="E60:E61" si="22">TEXT(B60,"00")&amp;IF(C60="","","-"&amp;TEXT(C60,"00"))&amp;IF(D60="","","-"&amp;TEXT(D60,"00"))</f>
+        <v>06-02-01</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>165</v>
@@ -3787,42 +3949,55 @@
         <v>23</v>
       </c>
       <c r="M60" s="1" t="str">
+        <f t="shared" ref="M60:M61" si="23">IF(I60="↑","",IF(I60="-","",System_Code&amp;"_"&amp;H60&amp;IF(L60="-","","_"&amp;L60)))</f>
+        <v/>
+      </c>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A61" s="1">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="B61" s="1">
+        <v>6</v>
+      </c>
+      <c r="C61" s="1">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>06-02-02</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M61" s="1" t="str">
         <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A61" s="1">
-        <f t="shared" si="3"/>
-        <v>57</v>
-      </c>
-      <c r="B61" s="1">
-        <v>6</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="6" t="str">
-        <f>TEXT(B61,"00")&amp;IF(C61="","","-"&amp;TEXT(C61,"00"))&amp;IF(D61="","",TEXT(D61,"00"))</f>
-        <v>06</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G61" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I61" s="7"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6"/>
-      <c r="N61" s="6"/>
-      <c r="O61" s="6"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62" s="1">
@@ -3833,35 +4008,37 @@
         <v>6</v>
       </c>
       <c r="C62" s="1">
-        <v>1</v>
-      </c>
-      <c r="D62" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>3</v>
+      </c>
       <c r="E62" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>06-01</v>
+        <f t="shared" si="20"/>
+        <v>06-02-03</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G62" s="15" t="s">
-        <v>97</v>
+        <v>178</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I62" s="4">
-        <v>8</v>
+        <v>165</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K62" s="1"/>
       <c r="L62" s="1" t="s">
-        <v>99</v>
+        <v>23</v>
       </c>
       <c r="M62" s="1" t="str">
-        <f t="shared" ref="M62:M70" si="24">IF(I62="↑","",IF(I62="-","",System_Code&amp;"_"&amp;H62&amp;IF(L62="-","","_"&amp;L62)))</f>
-        <v>SSE19_BD_SDD</v>
+        <f t="shared" si="21"/>
+        <v/>
       </c>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
@@ -3875,23 +4052,23 @@
         <v>6</v>
       </c>
       <c r="C63" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E63" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>06-01-01</v>
+        <f t="shared" si="20"/>
+        <v>06-02-04</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>94</v>
+        <v>185</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>23</v>
@@ -3904,7 +4081,7 @@
         <v>23</v>
       </c>
       <c r="M63" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="N63" s="1"/>
@@ -3919,23 +4096,23 @@
         <v>6</v>
       </c>
       <c r="C64" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D64" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E64" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>06-01-02</v>
+        <f t="shared" ref="E64:E65" si="24">TEXT(B64,"00")&amp;IF(C64="","","-"&amp;TEXT(C64,"00"))&amp;IF(D64="","","-"&amp;TEXT(D64,"00"))</f>
+        <v>06-02-05</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>89</v>
+        <v>165</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>23</v>
@@ -3948,7 +4125,7 @@
         <v>23</v>
       </c>
       <c r="M64" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="M64:M65" si="25">IF(I64="↑","",IF(I64="-","",System_Code&amp;"_"&amp;H64&amp;IF(L64="-","","_"&amp;L64)))</f>
         <v/>
       </c>
       <c r="N64" s="1"/>
@@ -3965,33 +4142,35 @@
       <c r="C65" s="1">
         <v>2</v>
       </c>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1">
+        <v>6</v>
+      </c>
       <c r="E65" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>06-02</v>
+        <f t="shared" si="24"/>
+        <v>06-02-06</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G65" s="15" t="s">
-        <v>96</v>
+        <v>181</v>
+      </c>
+      <c r="G65" s="16" t="s">
+        <v>187</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I65" s="4">
-        <v>8</v>
+        <v>165</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="M65" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>SSE19_BD_STD</v>
+        <f t="shared" si="25"/>
+        <v/>
       </c>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
@@ -4002,43 +4181,30 @@
         <v>62</v>
       </c>
       <c r="B66" s="1">
-        <v>6</v>
-      </c>
-      <c r="C66" s="1">
-        <v>3</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>06-03</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G66" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="H66" s="1" t="s">
+      <c r="E66" s="6" t="str">
+        <f>TEXT(B66,"00")&amp;IF(C66="","","-"&amp;TEXT(C66,"00"))&amp;IF(D66="","",TEXT(D66,"00"))</f>
+        <v>07</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G66" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H66" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="I66" s="4">
-        <v>8</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M66" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>SSE19_BD_RDD</v>
-      </c>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
+      <c r="O66" s="6"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
@@ -4046,21 +4212,21 @@
         <v>63</v>
       </c>
       <c r="B67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C67" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>06-04</v>
+        <v>07-01</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>89</v>
@@ -4073,11 +4239,11 @@
       </c>
       <c r="K67" s="1"/>
       <c r="L67" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="M67" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>SSE19_BD_IFD</v>
+        <f t="shared" ref="M67:M75" si="26">IF(I67="↑","",IF(I67="-","",System_Code&amp;"_"&amp;H67&amp;IF(L67="-","","_"&amp;L67)))</f>
+        <v>SSE19_BD_SDD</v>
       </c>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
@@ -4088,38 +4254,40 @@
         <v>64</v>
       </c>
       <c r="B68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C68" s="1">
-        <v>5</v>
-      </c>
-      <c r="D68" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D68" s="1">
+        <v>1</v>
+      </c>
       <c r="E68" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>06-05</v>
+        <v>07-01-01</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G68" s="15" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="G68" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I68" s="4">
-        <v>8</v>
+      <c r="I68" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K68" s="1"/>
       <c r="L68" s="1" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="M68" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>SSE19_BD_API</v>
+        <f t="shared" si="26"/>
+        <v/>
       </c>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -4130,38 +4298,40 @@
         <v>65</v>
       </c>
       <c r="B69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C69" s="1">
-        <v>6</v>
-      </c>
-      <c r="D69" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D69" s="1">
+        <v>2</v>
+      </c>
       <c r="E69" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>06-06</v>
+        <v>07-01-02</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G69" s="15" t="s">
-        <v>112</v>
+        <v>92</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I69" s="4">
-        <v>8</v>
+      <c r="I69" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K69" s="1"/>
       <c r="L69" s="1" t="s">
-        <v>110</v>
+        <v>23</v>
       </c>
       <c r="M69" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>SSE19_BD_BJD</v>
+        <f t="shared" si="26"/>
+        <v/>
       </c>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
@@ -4172,38 +4342,38 @@
         <v>66</v>
       </c>
       <c r="B70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C70" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>06-07</v>
+        <v>07-02</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="G70" s="15" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>89</v>
       </c>
       <c r="I70" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="M70" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>SSE19_BD_FL</v>
+        <f t="shared" si="26"/>
+        <v>SSE19_BD_STD</v>
       </c>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -4216,28 +4386,41 @@
       <c r="B71" s="1">
         <v>7</v>
       </c>
-      <c r="C71" s="1"/>
+      <c r="C71" s="1">
+        <v>3</v>
+      </c>
       <c r="D71" s="1"/>
-      <c r="E71" s="6" t="str">
-        <f>TEXT(B71,"00")&amp;IF(C71="","","-"&amp;TEXT(C71,"00"))&amp;IF(D71="","",TEXT(D71,"00"))</f>
-        <v>07</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I71" s="7"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
+      <c r="E71" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>07-03</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I71" s="4">
+        <v>8</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M71" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>SSE19_BD_RDD</v>
+      </c>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A72" s="1">
@@ -4248,21 +4431,21 @@
         <v>7</v>
       </c>
       <c r="C72" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-01</v>
+        <v>07-04</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="I72" s="4">
         <v>8</v>
@@ -4270,15 +4453,13 @@
       <c r="J72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K72" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="K72" s="1"/>
       <c r="L72" s="1" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="M72" s="1" t="str">
-        <f>IF(I72="↑","",IF(I72="-","",System_Code&amp;"_"&amp;H72&amp;IF(L72="-","","_"&amp;L72)))</f>
-        <v>SSE19_SD_ACHS</v>
+        <f t="shared" si="26"/>
+        <v>SSE19_BD_IFD</v>
       </c>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -4292,21 +4473,21 @@
         <v>7</v>
       </c>
       <c r="C73" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-02</v>
+        <v>07-05</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="I73" s="4">
         <v>8</v>
@@ -4314,15 +4495,13 @@
       <c r="J73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K73" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="K73" s="1"/>
       <c r="L73" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="M73" s="1" t="str">
-        <f>IF(I73="↑","",IF(I73="-","",System_Code&amp;"_"&amp;H73&amp;IF(L73="-","","_"&amp;L73)))</f>
-        <v>SSE19_SD_ACHA</v>
+        <f t="shared" si="26"/>
+        <v>SSE19_BD_API</v>
       </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -4336,37 +4515,35 @@
         <v>7</v>
       </c>
       <c r="C74" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="str">
-        <f t="shared" ref="E74" si="25">TEXT(B74,"00")&amp;IF(C74="","","-"&amp;TEXT(C74,"00"))&amp;IF(D74="","","-"&amp;TEXT(D74,"00"))</f>
-        <v>07-03</v>
+        <f t="shared" si="13"/>
+        <v>07-06</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>227</v>
+        <v>111</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>228</v>
+        <v>112</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="I74" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K74" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="K74" s="1"/>
       <c r="L74" s="1" t="s">
-        <v>229</v>
+        <v>110</v>
       </c>
       <c r="M74" s="1" t="str">
-        <f>IF(I74="↑","",IF(I74="-","",System_Code&amp;"_"&amp;H74&amp;IF(L74="-","","_"&amp;L74)))</f>
-        <v>SSE19_SD_ERD</v>
+        <f t="shared" si="26"/>
+        <v>SSE19_BD_BJD</v>
       </c>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -4380,21 +4557,21 @@
         <v>7</v>
       </c>
       <c r="C75" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-04</v>
+        <v>07-07</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="I75" s="4">
         <v>4</v>
@@ -4402,15 +4579,13 @@
       <c r="J75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K75" s="1" t="s">
-        <v>209</v>
-      </c>
+      <c r="K75" s="1"/>
       <c r="L75" s="1" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="M75" s="1" t="str">
-        <f>IF(I75="↑","",IF(I75="-","",System_Code&amp;"_"&amp;H75&amp;IF(L75="-","","_"&amp;L75)))</f>
-        <v>SSE19_SD_TBLD</v>
+        <f t="shared" si="26"/>
+        <v>SSE19_BD_FL</v>
       </c>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -4430,13 +4605,13 @@
         <v>08</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>225</v>
+        <v>116</v>
       </c>
       <c r="G76" s="14" t="s">
-        <v>226</v>
+        <v>117</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>241</v>
+        <v>118</v>
       </c>
       <c r="I76" s="7"/>
       <c r="J76" s="6"/>
@@ -4459,38 +4634,40 @@
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1" t="str">
-        <f t="shared" ref="E77:E78" si="26">TEXT(B77,"00")&amp;IF(C77="","","-"&amp;TEXT(C77,"00"))&amp;IF(D77="","","-"&amp;TEXT(D77,"00"))</f>
+        <f t="shared" si="13"/>
         <v>08-01</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="G77" s="15" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>241</v>
+        <v>118</v>
       </c>
       <c r="I77" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K77" s="1"/>
+      <c r="K77" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="L77" s="1" t="s">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="M77" s="1" t="str">
         <f>IF(I77="↑","",IF(I77="-","",System_Code&amp;"_"&amp;H77&amp;IF(L77="-","","_"&amp;L77)))</f>
-        <v>SSE19_Iter-pre_MVP</v>
+        <v>SSE19_SD_ACHS</v>
       </c>
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
-        <f t="shared" ref="A78:A105" si="27">ROW()-4</f>
+        <f t="shared" si="3"/>
         <v>74</v>
       </c>
       <c r="B78" s="1">
@@ -4501,31 +4678,33 @@
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="13"/>
         <v>08-02</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>241</v>
+        <v>118</v>
       </c>
       <c r="I78" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K78" s="1"/>
+      <c r="K78" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="L78" s="1" t="s">
-        <v>171</v>
+        <v>124</v>
       </c>
       <c r="M78" s="1" t="str">
         <f>IF(I78="↑","",IF(I78="-","",System_Code&amp;"_"&amp;H78&amp;IF(L78="-","","_"&amp;L78)))</f>
-        <v>SSE19_Iter-pre_PBL</v>
+        <v>SSE19_SD_ACHA</v>
       </c>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -4536,109 +4715,122 @@
         <v>75</v>
       </c>
       <c r="B79" s="1">
-        <v>9</v>
-      </c>
-      <c r="C79" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C79" s="1">
+        <v>3</v>
+      </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="6" t="str">
-        <f>TEXT(B79,"00")&amp;IF(C79="","","-"&amp;TEXT(C79,"00"))&amp;IF(D79="","",TEXT(D79,"00"))</f>
-        <v>09</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H79" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="I79" s="7"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6"/>
-      <c r="O79" s="6"/>
+      <c r="E79" s="1" t="str">
+        <f t="shared" ref="E79" si="27">TEXT(B79,"00")&amp;IF(C79="","","-"&amp;TEXT(C79,"00"))&amp;IF(D79="","","-"&amp;TEXT(D79,"00"))</f>
+        <v>08-03</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="G79" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I79" s="4">
+        <v>4</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M79" s="1" t="str">
+        <f>IF(I79="↑","",IF(I79="-","",System_Code&amp;"_"&amp;H79&amp;IF(L79="-","","_"&amp;L79)))</f>
+        <v>SSE19_SD_ERD</v>
+      </c>
+      <c r="N79" s="1"/>
+      <c r="O79" s="1"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A80" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
       <c r="B80" s="1">
-        <v>9</v>
-      </c>
-      <c r="C80" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C80" s="1">
+        <v>4</v>
+      </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09</v>
+        <v>08-04</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="G80" s="15" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>23</v>
+        <v>118</v>
+      </c>
+      <c r="I80" s="4">
+        <v>4</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="M80" s="1" t="str">
         <f>IF(I80="↑","",IF(I80="-","",System_Code&amp;"_"&amp;H80&amp;IF(L80="-","","_"&amp;L80)))</f>
-        <v/>
+        <v>SSE19_SD_TBLD</v>
       </c>
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A81" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
       <c r="B81" s="1">
         <v>9</v>
       </c>
-      <c r="C81" s="1">
-        <v>1</v>
-      </c>
-      <c r="D81" s="1">
-        <v>1</v>
-      </c>
-      <c r="E81" s="1" t="str">
-        <f t="shared" ref="E81" si="28">TEXT(B81,"00")&amp;IF(C81="","","-"&amp;TEXT(C81,"00"))&amp;IF(D81="","","-"&amp;TEXT(D81,"00"))</f>
-        <v>09-01-01</v>
-      </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I81" s="4">
-        <v>4</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
-      <c r="O81" s="1"/>
-    </row>
-    <row r="82" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="6" t="str">
+        <f>TEXT(B81,"00")&amp;IF(C81="","","-"&amp;TEXT(C81,"00"))&amp;IF(D81="","",TEXT(D81,"00"))</f>
+        <v>09</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I81" s="7"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="6"/>
+      <c r="O81" s="6"/>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="B82" s="1">
@@ -4647,19 +4839,19 @@
       <c r="C82" s="1">
         <v>1</v>
       </c>
-      <c r="D82" s="1">
-        <v>2</v>
-      </c>
+      <c r="D82" s="1"/>
       <c r="E82" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-01-02</v>
-      </c>
-      <c r="F82" s="1"/>
-      <c r="G82" s="16" t="s">
-        <v>142</v>
+        <f t="shared" ref="E82:E83" si="28">TEXT(B82,"00")&amp;IF(C82="","","-"&amp;TEXT(C82,"00"))&amp;IF(D82="","","-"&amp;TEXT(D82,"00"))</f>
+        <v>09-01</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>138</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I82" s="4">
         <v>4</v>
@@ -4668,35 +4860,40 @@
         <v>13</v>
       </c>
       <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-      <c r="M82" s="1"/>
+      <c r="L82" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="M82" s="1" t="str">
+        <f>IF(I82="↑","",IF(I82="-","",System_Code&amp;"_"&amp;H82&amp;IF(L82="-","","_"&amp;L82)))</f>
+        <v>SSE19_Iter-pre_MVP</v>
+      </c>
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="A83:A110" si="29">ROW()-4</f>
         <v>79</v>
       </c>
       <c r="B83" s="1">
         <v>9</v>
       </c>
       <c r="C83" s="1">
-        <v>1</v>
-      </c>
-      <c r="D83" s="1">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D83" s="1"/>
       <c r="E83" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-01-03</v>
-      </c>
-      <c r="F83" s="1"/>
-      <c r="G83" s="16" t="s">
-        <v>143</v>
+        <f t="shared" si="28"/>
+        <v>09-02</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I83" s="4">
         <v>4</v>
@@ -4705,106 +4902,106 @@
         <v>13</v>
       </c>
       <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
+      <c r="L83" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M83" s="1" t="str">
+        <f>IF(I83="↑","",IF(I83="-","",System_Code&amp;"_"&amp;H83&amp;IF(L83="-","","_"&amp;L83)))</f>
+        <v>SSE19_Iter-pre_PBL</v>
+      </c>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
       <c r="B84" s="1">
-        <v>9</v>
-      </c>
-      <c r="C84" s="1">
-        <v>1</v>
-      </c>
-      <c r="D84" s="1">
-        <v>4</v>
-      </c>
-      <c r="E84" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-01-04</v>
-      </c>
-      <c r="F84" s="1"/>
-      <c r="G84" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="6" t="str">
+        <f>TEXT(B84,"00")&amp;IF(C84="","","-"&amp;TEXT(C84,"00"))&amp;IF(D84="","",TEXT(D84,"00"))</f>
+        <v>10</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H84" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="I84" s="4">
-        <v>4</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
-      <c r="M84" s="1"/>
-      <c r="N84" s="1"/>
-      <c r="O84" s="1"/>
+      <c r="I84" s="7"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+      <c r="O84" s="6"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>81</v>
       </c>
       <c r="B85" s="1">
-        <v>9</v>
-      </c>
-      <c r="C85" s="1">
-        <v>1</v>
-      </c>
-      <c r="D85" s="1">
-        <v>5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
       <c r="E85" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-01-05</v>
-      </c>
-      <c r="F85" s="1"/>
-      <c r="G85" s="16" t="s">
-        <v>145</v>
+        <v>10</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>129</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="I85" s="4">
-        <v>4</v>
+      <c r="I85" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
+      <c r="M85" s="1" t="str">
+        <f>IF(I85="↑","",IF(I85="-","",System_Code&amp;"_"&amp;H85&amp;IF(L85="-","","_"&amp;L85)))</f>
+        <v/>
+      </c>
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A86" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>82</v>
       </c>
       <c r="B86" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C86" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D86" s="1">
         <v>1</v>
       </c>
       <c r="E86" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-02-01</v>
+        <f t="shared" ref="E86" si="30">TEXT(B86,"00")&amp;IF(C86="","","-"&amp;TEXT(C86,"00"))&amp;IF(D86="","","-"&amp;TEXT(D86,"00"))</f>
+        <v>10-01-01</v>
       </c>
       <c r="F86" s="1"/>
-      <c r="G86" s="16" t="s">
-        <v>146</v>
+      <c r="G86" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>240</v>
@@ -4821,27 +5018,27 @@
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>83</v>
       </c>
       <c r="B87" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C87" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" s="1">
         <v>2</v>
       </c>
       <c r="E87" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-02-02</v>
+        <v>10-01-02</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="16" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>240</v>
@@ -4860,25 +5057,25 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>84</v>
       </c>
       <c r="B88" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C88" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D88" s="1">
         <v>3</v>
       </c>
       <c r="E88" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-02-03</v>
+        <v>10-01-03</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="16" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>240</v>
@@ -4895,27 +5092,27 @@
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
     </row>
-    <row r="89" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>85</v>
       </c>
       <c r="B89" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" s="1">
         <v>4</v>
       </c>
       <c r="E89" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-02-04</v>
+        <v>10-01-04</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="16" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>240</v>
@@ -4934,25 +5131,25 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>86</v>
       </c>
       <c r="B90" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C90" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D90" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E90" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-03-01</v>
+        <v>10-01-05</v>
       </c>
       <c r="F90" s="1"/>
-      <c r="G90" s="13" t="s">
-        <v>150</v>
+      <c r="G90" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>240</v>
@@ -4969,27 +5166,27 @@
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
     </row>
-    <row r="91" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>87</v>
       </c>
       <c r="B91" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D91" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-03-02</v>
+        <v>10-02-01</v>
       </c>
       <c r="F91" s="1"/>
-      <c r="G91" s="13" t="s">
-        <v>151</v>
+      <c r="G91" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>240</v>
@@ -5008,25 +5205,25 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>88</v>
       </c>
       <c r="B92" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C92" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D92" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E92" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-03-03</v>
+        <v>10-02-02</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="16" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>240</v>
@@ -5043,27 +5240,27 @@
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
     </row>
-    <row r="93" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>89</v>
       </c>
       <c r="B93" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C93" s="1">
+        <v>2</v>
+      </c>
+      <c r="D93" s="1">
         <v>3</v>
-      </c>
-      <c r="D93" s="1">
-        <v>4</v>
       </c>
       <c r="E93" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-03-04</v>
+        <v>10-02-03</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="16" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>240</v>
@@ -5082,25 +5279,25 @@
     </row>
     <row r="94" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>90</v>
       </c>
       <c r="B94" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C94" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D94" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-03-05</v>
+        <v>10-02-04</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="16" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>240</v>
@@ -5119,25 +5316,25 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>91</v>
       </c>
       <c r="B95" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C95" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D95" s="1">
         <v>1</v>
       </c>
       <c r="E95" s="1" t="str">
-        <f>TEXT(B95,"00")&amp;IF(C95="","","-"&amp;TEXT(C95,"00"))&amp;IF(D95="","","-"&amp;TEXT(D95,"00"))</f>
-        <v>09-04-01</v>
+        <f t="shared" si="13"/>
+        <v>10-03-01</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="17" t="s">
-        <v>193</v>
+      <c r="G95" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>240</v>
@@ -5154,27 +5351,27 @@
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>92</v>
       </c>
       <c r="B96" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C96" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D96" s="1">
         <v>2</v>
       </c>
       <c r="E96" s="1" t="str">
-        <f>TEXT(B96,"00")&amp;IF(C96="","","-"&amp;TEXT(C96,"00"))&amp;IF(D96="","","-"&amp;TEXT(D96,"00"))</f>
-        <v>09-04-02</v>
+        <f t="shared" si="13"/>
+        <v>10-03-02</v>
       </c>
       <c r="F96" s="1"/>
-      <c r="G96" s="16" t="s">
-        <v>194</v>
+      <c r="G96" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>240</v>
@@ -5193,25 +5390,25 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>93</v>
       </c>
       <c r="B97" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C97" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D97" s="1">
         <v>3</v>
       </c>
       <c r="E97" s="1" t="str">
-        <f>TEXT(B97,"00")&amp;IF(C97="","","-"&amp;TEXT(C97,"00"))&amp;IF(D97="","","-"&amp;TEXT(D97,"00"))</f>
-        <v>09-04-03</v>
+        <f t="shared" si="13"/>
+        <v>10-03-03</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="16" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>240</v>
@@ -5230,25 +5427,25 @@
     </row>
     <row r="98" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>94</v>
       </c>
       <c r="B98" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C98" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D98" s="1">
         <v>4</v>
       </c>
       <c r="E98" s="1" t="str">
-        <f>TEXT(B98,"00")&amp;IF(C98="","","-"&amp;TEXT(C98,"00"))&amp;IF(D98="","","-"&amp;TEXT(D98,"00"))</f>
-        <v>09-04-04</v>
+        <f t="shared" si="13"/>
+        <v>10-03-04</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="16" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>240</v>
@@ -5265,27 +5462,27 @@
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>95</v>
       </c>
       <c r="B99" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C99" s="1">
+        <v>3</v>
+      </c>
+      <c r="D99" s="1">
         <v>5</v>
-      </c>
-      <c r="D99" s="1">
-        <v>1</v>
       </c>
       <c r="E99" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-05-01</v>
+        <v>10-03-05</v>
       </c>
       <c r="F99" s="1"/>
-      <c r="G99" s="13" t="s">
-        <v>197</v>
+      <c r="G99" s="16" t="s">
+        <v>154</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>240</v>
@@ -5302,27 +5499,27 @@
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>96</v>
       </c>
       <c r="B100" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C100" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D100" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E100" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-05-02</v>
+        <f>TEXT(B100,"00")&amp;IF(C100="","","-"&amp;TEXT(C100,"00"))&amp;IF(D100="","","-"&amp;TEXT(D100,"00"))</f>
+        <v>10-04-01</v>
       </c>
       <c r="F100" s="1"/>
-      <c r="G100" s="16" t="s">
-        <v>198</v>
+      <c r="G100" s="17" t="s">
+        <v>193</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>240</v>
@@ -5341,25 +5538,25 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>97</v>
       </c>
       <c r="B101" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C101" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D101" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E101" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-05-03</v>
+        <f>TEXT(B101,"00")&amp;IF(C101="","","-"&amp;TEXT(C101,"00"))&amp;IF(D101="","","-"&amp;TEXT(D101,"00"))</f>
+        <v>10-04-02</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="16" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>240</v>
@@ -5376,27 +5573,27 @@
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
     </row>
-    <row r="102" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>98</v>
       </c>
       <c r="B102" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C102" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D102" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E102" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-05-04</v>
+        <f>TEXT(B102,"00")&amp;IF(C102="","","-"&amp;TEXT(C102,"00"))&amp;IF(D102="","","-"&amp;TEXT(D102,"00"))</f>
+        <v>10-04-03</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="16" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>240</v>
@@ -5415,25 +5612,25 @@
     </row>
     <row r="103" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>99</v>
       </c>
       <c r="B103" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C103" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D103" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E103" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>09-05-05</v>
+        <f>TEXT(B103,"00")&amp;IF(C103="","","-"&amp;TEXT(C103,"00"))&amp;IF(D103="","","-"&amp;TEXT(D103,"00"))</f>
+        <v>10-04-04</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="16" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>240</v>
@@ -5450,27 +5647,27 @@
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
     </row>
-    <row r="104" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>100</v>
       </c>
       <c r="B104" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D104" s="1">
         <v>1</v>
       </c>
       <c r="E104" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-06-01</v>
+        <v>10-05-01</v>
       </c>
       <c r="F104" s="1"/>
-      <c r="G104" s="16" t="s">
-        <v>155</v>
+      <c r="G104" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>240</v>
@@ -5487,27 +5684,27 @@
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>101</v>
       </c>
       <c r="B105" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C105" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D105" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E105" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>09-07-01</v>
+        <v>10-05-02</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="16" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>240</v>
@@ -5525,34 +5722,275 @@
       <c r="O105" s="1"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="2"/>
-      <c r="N106" s="2"/>
-      <c r="O106" s="2"/>
+      <c r="A106" s="1">
+        <f t="shared" si="29"/>
+        <v>102</v>
+      </c>
+      <c r="B106" s="1">
+        <v>10</v>
+      </c>
+      <c r="C106" s="1">
+        <v>5</v>
+      </c>
+      <c r="D106" s="1">
+        <v>3</v>
+      </c>
+      <c r="E106" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-05-03</v>
+      </c>
+      <c r="F106" s="1"/>
+      <c r="G106" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I106" s="4">
+        <v>4</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K106" s="1"/>
+      <c r="L106" s="1"/>
+      <c r="M106" s="1"/>
+      <c r="N106" s="1"/>
+      <c r="O106" s="1"/>
+    </row>
+    <row r="107" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="A107" s="1">
+        <f t="shared" si="29"/>
+        <v>103</v>
+      </c>
+      <c r="B107" s="1">
+        <v>10</v>
+      </c>
+      <c r="C107" s="1">
+        <v>5</v>
+      </c>
+      <c r="D107" s="1">
+        <v>4</v>
+      </c>
+      <c r="E107" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-05-04</v>
+      </c>
+      <c r="F107" s="1"/>
+      <c r="G107" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I107" s="4">
+        <v>4</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K107" s="1"/>
+      <c r="L107" s="1"/>
+      <c r="M107" s="1"/>
+      <c r="N107" s="1"/>
+      <c r="O107" s="1"/>
+    </row>
+    <row r="108" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="A108" s="1">
+        <f t="shared" si="29"/>
+        <v>104</v>
+      </c>
+      <c r="B108" s="1">
+        <v>10</v>
+      </c>
+      <c r="C108" s="1">
+        <v>5</v>
+      </c>
+      <c r="D108" s="1">
+        <v>5</v>
+      </c>
+      <c r="E108" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-05-05</v>
+      </c>
+      <c r="F108" s="1"/>
+      <c r="G108" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I108" s="4">
+        <v>4</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K108" s="1"/>
+      <c r="L108" s="1"/>
+      <c r="M108" s="1"/>
+      <c r="N108" s="1"/>
+      <c r="O108" s="1"/>
+    </row>
+    <row r="109" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="A109" s="1">
+        <f t="shared" si="29"/>
+        <v>105</v>
+      </c>
+      <c r="B109" s="1">
+        <v>10</v>
+      </c>
+      <c r="C109" s="1">
+        <v>6</v>
+      </c>
+      <c r="D109" s="1">
+        <v>1</v>
+      </c>
+      <c r="E109" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-06-01</v>
+      </c>
+      <c r="F109" s="1"/>
+      <c r="G109" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I109" s="4">
+        <v>4</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K109" s="1"/>
+      <c r="L109" s="1"/>
+      <c r="M109" s="1"/>
+      <c r="N109" s="1"/>
+      <c r="O109" s="1"/>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A110" s="1">
+        <f t="shared" si="29"/>
+        <v>106</v>
+      </c>
+      <c r="B110" s="1">
+        <v>10</v>
+      </c>
+      <c r="C110" s="1">
+        <v>7</v>
+      </c>
+      <c r="D110" s="1">
+        <v>1</v>
+      </c>
+      <c r="E110" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-07-01</v>
+      </c>
+      <c r="F110" s="1"/>
+      <c r="G110" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I110" s="4">
+        <v>4</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K110" s="1"/>
+      <c r="L110" s="1"/>
+      <c r="M110" s="1"/>
+      <c r="N110" s="1"/>
+      <c r="O110" s="1"/>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+      <c r="H111" s="2"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="2"/>
+      <c r="K111" s="2"/>
+      <c r="L111" s="2"/>
+      <c r="M111" s="2"/>
+      <c r="N111" s="2"/>
+      <c r="O111" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:O4" xr:uid="{93992286-983A-43C0-B01F-316812382256}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K6:K23 K25:K106">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="K6:K22 K29:K49 K55:K111">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K27">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K28">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K50:K51">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K52:K54">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>

</xml_diff>

<commit_message>
modify Biz and WBS
</commit_message>
<xml_diff>
--- a/_project_docs/SSE19_SPP_WBS.xlsx
+++ b/_project_docs/SSE19_SPP_WBS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\workplace\smartse19\_project_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED3B7D-B2F6-4762-A613-9DEF7C856660}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3418B158-7B6B-4FF6-B207-C72E60C1B781}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{D3C1DD7E-20E6-4452-8E15-DB8203761C57}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="263">
   <si>
     <t>No</t>
   </si>
@@ -181,9 +181,6 @@
     <t>イノベーション設計</t>
   </si>
   <si>
-    <t>INNOD</t>
-  </si>
-  <si>
     <t xml:space="preserve">Project Control </t>
   </si>
   <si>
@@ -337,9 +334,6 @@
     <t>STD</t>
   </si>
   <si>
-    <t>SDD</t>
-  </si>
-  <si>
     <t>UXD</t>
   </si>
   <si>
@@ -409,12 +403,6 @@
     <t>アプリケーション・アーキテクチャ設計</t>
   </si>
   <si>
-    <t>ACHS</t>
-  </si>
-  <si>
-    <t>ACHA</t>
-  </si>
-  <si>
     <t>Smart SE 2019-19 修了制作：働き方バランスアップサービス開発</t>
   </si>
   <si>
@@ -460,9 +448,6 @@
     <t>List up back log list</t>
   </si>
   <si>
-    <t>プロダクト・バックログ、スプリントバックログを決める</t>
-  </si>
-  <si>
     <t>1.1 GPS位置データを取得する（センサー側）</t>
   </si>
   <si>
@@ -604,12 +589,6 @@
     <t>Yさん</t>
   </si>
   <si>
-    <t>CUSTD</t>
-  </si>
-  <si>
-    <t>CUST_IV</t>
-  </si>
-  <si>
     <t>サービス提案（仮説）</t>
   </si>
   <si>
@@ -772,9 +751,6 @@
     <t>Validation for Prototyping</t>
   </si>
   <si>
-    <t>VALID</t>
-  </si>
-  <si>
     <t>keystrokes</t>
   </si>
   <si>
@@ -790,13 +766,67 @@
     <t>検証用プロトタイプ</t>
   </si>
   <si>
-    <t>activewindow</t>
-  </si>
-  <si>
     <t>pcactiveinfo</t>
   </si>
   <si>
     <t>PC Monitoringデータを加工</t>
+  </si>
+  <si>
+    <t>REQD</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>ペルソナ</t>
+  </si>
+  <si>
+    <t>Customer Interview</t>
+  </si>
+  <si>
+    <t>顧客インタビュー</t>
+  </si>
+  <si>
+    <t>INTERVIEW</t>
+  </si>
+  <si>
+    <t>PROTO</t>
+  </si>
+  <si>
+    <t>PROTD_keystrokes</t>
+  </si>
+  <si>
+    <t>PROTD_activewindow</t>
+  </si>
+  <si>
+    <t>PROTD_pcactiveinfo</t>
+  </si>
+  <si>
+    <t>ARCA</t>
+  </si>
+  <si>
+    <t>ARCS</t>
+  </si>
+  <si>
+    <t>対象外</t>
+  </si>
+  <si>
+    <t>SDD_01_Dashboard</t>
+  </si>
+  <si>
+    <t>SDD_00_Menu</t>
+  </si>
+  <si>
+    <t>List up sprint log list</t>
+  </si>
+  <si>
+    <t>プロダクト・バックログを決める</t>
+  </si>
+  <si>
+    <t>スプリントバックログを決める</t>
+  </si>
+  <si>
+    <t>SBL</t>
   </si>
 </sst>
 </file>
@@ -968,35 +998,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -1450,13 +1452,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O111"/>
+  <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M54" sqref="M54"/>
+      <selection pane="bottomRight" activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1476,14 +1478,14 @@
   <sheetData>
     <row r="1" spans="1:15" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C1" s="11"/>
       <c r="J1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="K1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -1495,7 +1497,7 @@
       </c>
       <c r="G2" s="9"/>
       <c r="K2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O2" s="12">
         <v>43697</v>
@@ -1538,7 +1540,7 @@
         <v>10</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>18</v>
@@ -1568,13 +1570,13 @@
         <v>01</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="6"/>
@@ -1604,10 +1606,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I6" s="4">
         <v>12</v>
@@ -1616,7 +1618,7 @@
         <v>13</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>19</v>
@@ -1648,10 +1650,10 @@
         <v>21</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I7" s="4">
         <v>12</v>
@@ -1660,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>20</v>
@@ -1705,7 +1707,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <f t="shared" ref="A9:A84" si="3">ROW()-4</f>
+        <f t="shared" ref="A9:A85" si="3">ROW()-4</f>
         <v>5</v>
       </c>
       <c r="B9" s="1">
@@ -1735,7 +1737,7 @@
         <v>13</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>23</v>
@@ -1779,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>24</v>
@@ -1823,7 +1825,7 @@
         <v>13</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>26</v>
@@ -1855,7 +1857,7 @@
         <v>31</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>12</v>
@@ -1867,7 +1869,7 @@
         <v>13</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>32</v>
@@ -1911,7 +1913,7 @@
         <v>13</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>35</v>
@@ -1940,10 +1942,10 @@
         <v>02-06</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>12</v>
@@ -1954,7 +1956,9 @@
       <c r="J14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="L14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -1999,10 +2003,10 @@
         <v>13</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M15" s="1" t="str">
         <f t="shared" si="5"/>
@@ -2033,7 +2037,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>12</v>
@@ -2044,9 +2048,11 @@
       <c r="J16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="L16" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="M16" s="1" t="str">
         <f t="shared" si="5"/>
@@ -2077,7 +2083,7 @@
         <v>38</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>12</v>
@@ -2088,9 +2094,11 @@
       <c r="J17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="L17" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M17" s="1" t="str">
         <f t="shared" si="5"/>
@@ -2118,10 +2126,10 @@
         <v>02-07-04</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>12</v>
@@ -2132,9 +2140,11 @@
       <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="L18" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="M18" s="1" t="str">
         <f t="shared" ref="M18" si="8">IF(I18="↑","",IF(I18="-","",System_Code&amp;"_"&amp;H18&amp;IF(L18="-","","_"&amp;L18)))</f>
@@ -2165,7 +2175,7 @@
         <v>39</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>12</v>
@@ -2177,7 +2187,7 @@
         <v>13</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>40</v>
@@ -2208,10 +2218,10 @@
         <v>02-07-06</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>12</v>
@@ -2223,10 +2233,10 @@
         <v>13</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="M20" s="1" t="str">
         <f t="shared" ref="M20" si="10">IF(I20="↑","",IF(I20="-","",System_Code&amp;"_"&amp;H20&amp;IF(L20="-","","_"&amp;L20)))</f>
@@ -2254,10 +2264,10 @@
         <v>02-07-07</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>12</v>
@@ -2269,7 +2279,7 @@
         <v>13</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>30</v>
@@ -2296,13 +2306,13 @@
         <v>03</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="6"/>
@@ -2335,7 +2345,7 @@
         <v>46</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I23" s="4">
         <v>8</v>
@@ -2344,14 +2354,14 @@
         <v>13</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>131</v>
+        <v>23</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="M23" s="1" t="str">
-        <f t="shared" ref="M23:M49" si="11">IF(I23="↑","",IF(I23="-","",System_Code&amp;"_"&amp;H23&amp;IF(L23="-","","_"&amp;L23)))</f>
-        <v>SSE19_Biz_INNOD</v>
+        <f>IF(I23="↑","",IF(I23="-","",System_Code&amp;"_"&amp;H23&amp;IF(L23="-","","_"&amp;L23)))</f>
+        <v>SSE19_Biz</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -2375,28 +2385,28 @@
         <v>03-01-01</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M24" s="1" t="str">
-        <f t="shared" ref="M24" si="12">IF(I24="↑","",IF(I24="-","",System_Code&amp;"_"&amp;H24&amp;IF(L24="-","","_"&amp;L24)))</f>
+        <f t="shared" ref="M24" si="11">IF(I24="↑","",IF(I24="-","",System_Code&amp;"_"&amp;H24&amp;IF(L24="-","","_"&amp;L24)))</f>
         <v/>
       </c>
       <c r="N24" s="1"/>
@@ -2421,28 +2431,28 @@
         <v>03-01-02</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="H25" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I25" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>52</v>
-      </c>
       <c r="J25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M25" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M25:M50" si="12">IF(I25="↑","",IF(I25="-","",System_Code&amp;"_"&amp;H25&amp;IF(L25="-","","_"&amp;L25)))</f>
         <v/>
       </c>
       <c r="N25" s="1"/>
@@ -2463,32 +2473,32 @@
         <v>3</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f t="shared" ref="E26:E110" si="13">TEXT(B26,"00")&amp;IF(C26="","","-"&amp;TEXT(C26,"00"))&amp;IF(D26="","","-"&amp;TEXT(D26,"00"))</f>
+        <f t="shared" ref="E26:E112" si="13">TEXT(B26,"00")&amp;IF(C26="","","-"&amp;TEXT(C26,"00"))&amp;IF(D26="","","-"&amp;TEXT(D26,"00"))</f>
         <v>03-01-03</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M26" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="N26" s="1"/>
@@ -2513,28 +2523,28 @@
         <v>03-01-04</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>56</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M27" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="N27" s="1"/>
@@ -2559,28 +2569,28 @@
         <v>03-01-05</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>64</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M28" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="N28" s="1"/>
@@ -2634,29 +2644,29 @@
         <v>04-02</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="4">
-        <v>8</v>
+      <c r="I30" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>136</v>
+        <v>23</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M30" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>SSE19_RD</v>
+        <f t="shared" si="12"/>
+        <v/>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2680,27 +2690,29 @@
         <v>04-02-01</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>60</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="10" t="s">
-        <v>52</v>
+      <c r="I31" s="10">
+        <v>4</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K31" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L31" s="1" t="s">
-        <v>23</v>
+        <v>244</v>
       </c>
       <c r="M31" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_REQD</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -2724,10 +2736,10 @@
         <v>04-02-02</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="16" t="s">
         <v>61</v>
-      </c>
-      <c r="G32" s="16" t="s">
-        <v>62</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>42</v>
@@ -2739,13 +2751,13 @@
         <v>13</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M32" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_REQL</v>
       </c>
       <c r="N32" s="1"/>
@@ -2768,10 +2780,10 @@
         <v>04-03</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>68</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>42</v>
@@ -2782,12 +2794,14 @@
       <c r="J33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="K33" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="L33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M33" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="N33" s="1"/>
@@ -2808,32 +2822,32 @@
         <v>1</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="E34" si="15">TEXT(B34,"00")&amp;IF(C34="","","-"&amp;TEXT(C34,"00"))&amp;IF(D34="","","-"&amp;TEXT(D34,"00"))</f>
         <v>04-03-01</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>69</v>
+        <v>245</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>70</v>
+        <v>246</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I34" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M34" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="M34" si="16">IF(I34="↑","",IF(I34="-","",System_Code&amp;"_"&amp;H34&amp;IF(L34="-","","_"&amp;L34)))</f>
         <v>SSE19_RD_UXD</v>
       </c>
       <c r="N34" s="1"/>
@@ -2858,28 +2872,28 @@
         <v>04-03-02</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G35" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I35" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M35" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_UXD</v>
       </c>
       <c r="N35" s="1"/>
@@ -2894,35 +2908,39 @@
         <v>4</v>
       </c>
       <c r="C36" s="1">
-        <v>4</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="D36" s="1">
+        <v>3</v>
+      </c>
       <c r="E36" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04</v>
+        <v>04-03-03</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>23</v>
+      <c r="I36" s="4">
+        <v>4</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="L36" s="1" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="M36" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_UXD</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2938,35 +2956,33 @@
       <c r="C37" s="1">
         <v>4</v>
       </c>
-      <c r="D37" s="1">
-        <v>1</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-01</v>
+        <v>04-04</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>202</v>
+        <v>72</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I37" s="4">
-        <v>4</v>
+      <c r="I37" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="1" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="M37" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>SSE19_RD_USD</v>
+        <f t="shared" si="12"/>
+        <v/>
       </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -2983,33 +2999,35 @@
         <v>4</v>
       </c>
       <c r="D38" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-02</v>
+        <v>04-04-01</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G38" s="16" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I38" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K38" s="1"/>
+      <c r="K38" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L38" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M38" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_USD</v>
       </c>
       <c r="N38" s="1"/>
@@ -3027,33 +3045,35 @@
         <v>4</v>
       </c>
       <c r="D39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-03</v>
+        <v>04-04-02</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I39" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L39" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M39" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_USD</v>
       </c>
       <c r="N39" s="1"/>
@@ -3071,33 +3091,35 @@
         <v>4</v>
       </c>
       <c r="D40" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-04</v>
+        <v>04-04-03</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>204</v>
+        <v>74</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I40" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="1"/>
+      <c r="K40" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L40" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M40" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_USD</v>
       </c>
       <c r="N40" s="1"/>
@@ -3115,33 +3137,35 @@
         <v>4</v>
       </c>
       <c r="D41" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-05</v>
+        <v>04-04-04</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I41" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="1"/>
+      <c r="K41" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L41" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M41" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_USD</v>
       </c>
       <c r="N41" s="1"/>
@@ -3159,17 +3183,17 @@
         <v>4</v>
       </c>
       <c r="D42" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-06</v>
+        <v>04-04-05</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>83</v>
+        <v>185</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>42</v>
@@ -3180,12 +3204,14 @@
       <c r="J42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K42" s="1"/>
+      <c r="K42" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L42" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M42" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>SSE19_RD_USD</v>
       </c>
       <c r="N42" s="1"/>
@@ -3203,17 +3229,17 @@
         <v>4</v>
       </c>
       <c r="D43" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E43" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>04-04-07</v>
+        <v>04-04-06</v>
       </c>
       <c r="F43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="16" t="s">
         <v>82</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>42</v>
@@ -3224,13 +3250,15 @@
       <c r="J43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="1"/>
+      <c r="K43" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L43" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M43" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>SSE19_RD_USD_OP</v>
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_USD</v>
       </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
@@ -3244,35 +3272,39 @@
         <v>4</v>
       </c>
       <c r="C44" s="1">
-        <v>5</v>
-      </c>
-      <c r="D44" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>7</v>
+      </c>
       <c r="E44" s="1" t="str">
-        <f t="shared" ref="E44:E48" si="15">TEXT(B44,"00")&amp;IF(C44="","","-"&amp;TEXT(C44,"00"))&amp;IF(D44="","","-"&amp;TEXT(D44,"00"))</f>
-        <v>04-05</v>
+        <f t="shared" si="13"/>
+        <v>04-04-07</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>158</v>
+        <v>81</v>
+      </c>
+      <c r="G44" s="16" t="s">
+        <v>83</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>23</v>
+      <c r="I44" s="4">
+        <v>4</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="L44" s="1" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="M44" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v/>
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_USD_OP</v>
       </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
@@ -3288,37 +3320,35 @@
       <c r="C45" s="1">
         <v>5</v>
       </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>04-05-01</v>
+        <f t="shared" ref="E45:E49" si="17">TEXT(B45,"00")&amp;IF(C45="","","-"&amp;TEXT(C45,"00"))&amp;IF(D45="","","-"&amp;TEXT(D45,"00"))</f>
+        <v>04-05</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>162</v>
+        <v>152</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>153</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I45" s="4">
-        <v>4</v>
+      <c r="I45" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="M45" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>SSE19_RD_CD</v>
+        <f t="shared" si="12"/>
+        <v/>
       </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
@@ -3335,17 +3365,17 @@
         <v>5</v>
       </c>
       <c r="D46" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>04-05-02</v>
+        <f t="shared" si="17"/>
+        <v>04-05-01</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G46" s="16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>42</v>
@@ -3357,14 +3387,14 @@
         <v>13</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="M46" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>SSE19_RD_CRD</v>
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_CD</v>
       </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
@@ -3381,17 +3411,17 @@
         <v>5</v>
       </c>
       <c r="D47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>04-05-03</v>
+        <f t="shared" si="17"/>
+        <v>04-05-02</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G47" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>42</v>
@@ -3403,14 +3433,14 @@
         <v>13</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>207</v>
+        <v>128</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="M47" s="1" t="str">
-        <f t="shared" ref="M47:M48" si="16">IF(I47="↑","",IF(I47="-","",System_Code&amp;"_"&amp;H47&amp;IF(L47="-","","_"&amp;L47)))</f>
-        <v>SSE19_RD_DFD</v>
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_CRD</v>
       </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
@@ -3427,17 +3457,17 @@
         <v>5</v>
       </c>
       <c r="D48" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f t="shared" si="15"/>
-        <v>04-05-04</v>
+        <f t="shared" si="17"/>
+        <v>04-05-03</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>230</v>
+        <v>156</v>
       </c>
       <c r="G48" s="16" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>42</v>
@@ -3449,14 +3479,14 @@
         <v>13</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>231</v>
+        <v>159</v>
       </c>
       <c r="M48" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>SSE19_RD_DFS</v>
+        <f t="shared" ref="M48:M49" si="18">IF(I48="↑","",IF(I48="-","",System_Code&amp;"_"&amp;H48&amp;IF(L48="-","","_"&amp;L48)))</f>
+        <v>SSE19_RD_DFD</v>
       </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
@@ -3473,17 +3503,17 @@
         <v>5</v>
       </c>
       <c r="D49" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f t="shared" ref="E49" si="17">TEXT(B49,"00")&amp;IF(C49="","","-"&amp;TEXT(C49,"00"))&amp;IF(D49="","","-"&amp;TEXT(D49,"00"))</f>
-        <v>04-05-05</v>
+        <f t="shared" si="17"/>
+        <v>04-05-04</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>42</v>
@@ -3495,14 +3525,14 @@
         <v>13</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>132</v>
+        <v>200</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="M49" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>SSE19_RD_DSM</v>
+        <f t="shared" si="18"/>
+        <v>SSE19_RD_DFS</v>
       </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
@@ -3513,28 +3543,45 @@
         <v>46</v>
       </c>
       <c r="B50" s="1">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
         <v>5</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="6" t="str">
-        <f>TEXT(B50,"00")&amp;IF(C50="","","-"&amp;TEXT(C50,"00"))&amp;IF(D50="","",TEXT(D50,"00"))</f>
-        <v>05</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="H50" s="6"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
+      <c r="D50" s="1">
+        <v>5</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <f t="shared" ref="E50" si="19">TEXT(B50,"00")&amp;IF(C50="","","-"&amp;TEXT(C50,"00"))&amp;IF(D50="","","-"&amp;TEXT(D50,"00"))</f>
+        <v>04-05-05</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I50" s="4">
+        <v>4</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M50" s="1" t="str">
+        <f t="shared" si="12"/>
+        <v>SSE19_RD_DSM</v>
+      </c>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
@@ -3544,33 +3591,28 @@
       <c r="B51" s="1">
         <v>5</v>
       </c>
-      <c r="C51" s="1">
-        <v>1</v>
-      </c>
+      <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="1" t="str">
-        <f t="shared" ref="E51:E54" si="18">TEXT(B51,"00")&amp;IF(C51="","","-"&amp;TEXT(C51,"00"))&amp;IF(D51="","","-"&amp;TEXT(D51,"00"))</f>
-        <v>05-01</v>
-      </c>
-      <c r="F51" s="1"/>
-      <c r="G51" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1" t="str">
-        <f>IF(I51="↑","",IF(I51="-","",System_Code&amp;"_"&amp;H51&amp;IF(L51="-","","_"&amp;L51)))</f>
-        <v/>
-      </c>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
+      <c r="E51" s="6" t="str">
+        <f>TEXT(B51,"00")&amp;IF(C51="","","-"&amp;TEXT(C51,"00"))&amp;IF(D51="","",TEXT(D51,"00"))</f>
+        <v>05</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="G51" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
@@ -3581,37 +3623,35 @@
         <v>5</v>
       </c>
       <c r="C52" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>05-02</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>245</v>
-      </c>
+        <f t="shared" ref="E52:E55" si="20">TEXT(B52,"00")&amp;IF(C52="","","-"&amp;TEXT(C52,"00"))&amp;IF(D52="","","-"&amp;TEXT(D52,"00"))</f>
+        <v>05-01</v>
+      </c>
+      <c r="F52" s="1"/>
       <c r="G52" s="15" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="I52" s="4">
-        <v>12</v>
+        <v>160</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>207</v>
+        <v>23</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>245</v>
+        <v>23</v>
       </c>
       <c r="M52" s="1" t="str">
         <f>IF(I52="↑","",IF(I52="-","",System_Code&amp;"_"&amp;H52&amp;IF(L52="-","","_"&amp;L52)))</f>
-        <v>SSE19_VALID_keystrokes</v>
+        <v/>
       </c>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -3625,21 +3665,23 @@
         <v>5</v>
       </c>
       <c r="C53" s="1">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
       <c r="E53" s="1" t="str">
-        <f t="shared" ref="E53" si="19">TEXT(B53,"00")&amp;IF(C53="","","-"&amp;TEXT(C53,"00"))&amp;IF(D53="","","-"&amp;TEXT(D53,"00"))</f>
-        <v>05-03</v>
+        <f t="shared" si="20"/>
+        <v>05-01-01</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>244</v>
+        <v>160</v>
       </c>
       <c r="I53" s="4">
         <v>12</v>
@@ -3648,14 +3690,14 @@
         <v>13</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M53" s="1" t="str">
         <f>IF(I53="↑","",IF(I53="-","",System_Code&amp;"_"&amp;H53&amp;IF(L53="-","","_"&amp;L53)))</f>
-        <v>SSE19_VALID_activewindow</v>
+        <v>SSE19_CD_PROTD_keystrokes</v>
       </c>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -3669,21 +3711,23 @@
         <v>5</v>
       </c>
       <c r="C54" s="1">
-        <v>4</v>
-      </c>
-      <c r="D54" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D54" s="1">
+        <v>2</v>
+      </c>
       <c r="E54" s="1" t="str">
-        <f t="shared" si="18"/>
-        <v>05-04</v>
+        <f t="shared" ref="E54" si="21">TEXT(B54,"00")&amp;IF(C54="","","-"&amp;TEXT(C54,"00"))&amp;IF(D54="","","-"&amp;TEXT(D54,"00"))</f>
+        <v>05-01-02</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>244</v>
+        <v>160</v>
       </c>
       <c r="I54" s="4">
         <v>12</v>
@@ -3692,14 +3736,14 @@
         <v>13</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M54" s="1" t="str">
         <f>IF(I54="↑","",IF(I54="-","",System_Code&amp;"_"&amp;H54&amp;IF(L54="-","","_"&amp;L54)))</f>
-        <v>SSE19_VALID_pcactiveinfo</v>
+        <v>SSE19_CD_PROTD_activewindow</v>
       </c>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -3710,30 +3754,45 @@
         <v>51</v>
       </c>
       <c r="B55" s="1">
-        <v>6</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="6" t="str">
-        <f>TEXT(B55,"00")&amp;IF(C55="","","-"&amp;TEXT(C55,"00"))&amp;IF(D55="","",TEXT(D55,"00"))</f>
-        <v>06</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
-      <c r="O55" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <f t="shared" si="20"/>
+        <v>05-01-03</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I55" s="4">
+        <v>12</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M55" s="1" t="str">
+        <f>IF(I55="↑","",IF(I55="-","",System_Code&amp;"_"&amp;H55&amp;IF(L55="-","","_"&amp;L55)))</f>
+        <v>SSE19_CD_PROTD_pcactiveinfo</v>
+      </c>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56" s="1">
@@ -3743,39 +3802,28 @@
       <c r="B56" s="1">
         <v>6</v>
       </c>
-      <c r="C56" s="1">
-        <v>1</v>
-      </c>
+      <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1" t="str">
-        <f t="shared" ref="E56:E63" si="20">TEXT(B56,"00")&amp;IF(C56="","","-"&amp;TEXT(C56,"00"))&amp;IF(D56="","","-"&amp;TEXT(D56,"00"))</f>
-        <v>06-01</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G56" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I56" s="4">
-        <v>8</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="M56" s="1" t="str">
-        <f t="shared" ref="M56:M63" si="21">IF(I56="↑","",IF(I56="-","",System_Code&amp;"_"&amp;H56&amp;IF(L56="-","","_"&amp;L56)))</f>
-        <v>SSE19_CD_CUSTD</v>
-      </c>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
+      <c r="E56" s="6" t="str">
+        <f>TEXT(B56,"00")&amp;IF(C56="","","-"&amp;TEXT(C56,"00"))&amp;IF(D56="","",TEXT(D56,"00"))</f>
+        <v>06</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="H56" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I56" s="7"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57" s="1">
@@ -3788,36 +3836,34 @@
       <c r="C57" s="1">
         <v>1</v>
       </c>
-      <c r="D57" s="1">
-        <v>1</v>
-      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v>06-01-01</v>
+        <f t="shared" ref="E57:E64" si="22">TEXT(B57,"00")&amp;IF(C57="","","-"&amp;TEXT(C57,"00"))&amp;IF(D57="","","-"&amp;TEXT(D57,"00"))</f>
+        <v>06-01</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G57" s="16" t="s">
-        <v>94</v>
+        <v>169</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>170</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I57" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J57" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="L57" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M57" s="1" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="M57:M64" si="23">IF(I57="↑","",IF(I57="-","",System_Code&amp;"_"&amp;H57&amp;IF(L57="-","","_"&amp;L57)))</f>
         <v/>
       </c>
       <c r="N57" s="1"/>
@@ -3835,36 +3881,36 @@
         <v>1</v>
       </c>
       <c r="D58" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v>06-01-02</v>
+        <f t="shared" si="22"/>
+        <v>06-01-01</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>23</v>
+        <v>160</v>
+      </c>
+      <c r="I58" s="4">
+        <v>6</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>23</v>
+        <v>250</v>
       </c>
       <c r="M58" s="1" t="str">
-        <f t="shared" si="21"/>
-        <v/>
+        <f t="shared" si="23"/>
+        <v>SSE19_CD_PROTO</v>
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -3878,35 +3924,39 @@
         <v>6</v>
       </c>
       <c r="C59" s="1">
+        <v>1</v>
+      </c>
+      <c r="D59" s="1">
         <v>2</v>
       </c>
-      <c r="D59" s="1"/>
       <c r="E59" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v>06-02</v>
+        <f t="shared" si="22"/>
+        <v>06-01-02</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G59" s="15" t="s">
-        <v>173</v>
+        <v>91</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I59" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K59" s="1"/>
+      <c r="K59" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="L59" s="1" t="s">
-        <v>189</v>
+        <v>250</v>
       </c>
       <c r="M59" s="1" t="str">
-        <f t="shared" si="21"/>
-        <v>SSE19_CD_CUST_IV</v>
+        <f t="shared" si="23"/>
+        <v>SSE19_CD_PROTO</v>
       </c>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
@@ -3922,35 +3972,33 @@
       <c r="C60" s="1">
         <v>2</v>
       </c>
-      <c r="D60" s="1">
-        <v>1</v>
-      </c>
+      <c r="D60" s="1"/>
       <c r="E60" s="1" t="str">
-        <f t="shared" ref="E60:E61" si="22">TEXT(B60,"00")&amp;IF(C60="","","-"&amp;TEXT(C60,"00"))&amp;IF(D60="","","-"&amp;TEXT(D60,"00"))</f>
-        <v>06-02-01</v>
+        <f t="shared" si="22"/>
+        <v>06-02</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>182</v>
+        <v>247</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>248</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>23</v>
+        <v>160</v>
+      </c>
+      <c r="I60" s="4">
+        <v>10</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="K60" s="1"/>
       <c r="L60" s="1" t="s">
-        <v>23</v>
+        <v>249</v>
       </c>
       <c r="M60" s="1" t="str">
-        <f t="shared" ref="M60:M61" si="23">IF(I60="↑","",IF(I60="-","",System_Code&amp;"_"&amp;H60&amp;IF(L60="-","","_"&amp;L60)))</f>
-        <v/>
+        <f t="shared" si="23"/>
+        <v>SSE19_CD_INTERVIEW</v>
       </c>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -3967,20 +4015,20 @@
         <v>2</v>
       </c>
       <c r="D61" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E61" s="1" t="str">
-        <f t="shared" si="22"/>
-        <v>06-02-02</v>
+        <f t="shared" ref="E61:E62" si="24">TEXT(B61,"00")&amp;IF(C61="","","-"&amp;TEXT(C61,"00"))&amp;IF(D61="","","-"&amp;TEXT(D61,"00"))</f>
+        <v>06-02-01</v>
       </c>
       <c r="F61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G61" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="G61" s="16" t="s">
-        <v>183</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>23</v>
@@ -3993,97 +4041,97 @@
         <v>23</v>
       </c>
       <c r="M61" s="1" t="str">
+        <f t="shared" ref="M61:M62" si="25">IF(I61="↑","",IF(I61="-","",System_Code&amp;"_"&amp;H61&amp;IF(L61="-","","_"&amp;L61)))</f>
+        <v/>
+      </c>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A62" s="1">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B62" s="1">
+        <v>6</v>
+      </c>
+      <c r="C62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>06-02-02</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M62" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A63" s="1">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="B63" s="1">
+        <v>6</v>
+      </c>
+      <c r="C63" s="1">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>06-02-03</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G63" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M63" s="1" t="str">
         <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A62" s="1">
-        <f t="shared" si="3"/>
-        <v>58</v>
-      </c>
-      <c r="B62" s="1">
-        <v>6</v>
-      </c>
-      <c r="C62" s="1">
-        <v>2</v>
-      </c>
-      <c r="D62" s="1">
-        <v>3</v>
-      </c>
-      <c r="E62" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v>06-02-03</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="H62" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I62" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M62" s="1" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A63" s="1">
-        <f t="shared" si="3"/>
-        <v>59</v>
-      </c>
-      <c r="B63" s="1">
-        <v>6</v>
-      </c>
-      <c r="C63" s="1">
-        <v>2</v>
-      </c>
-      <c r="D63" s="1">
-        <v>4</v>
-      </c>
-      <c r="E63" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v>06-02-04</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M63" s="1" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
@@ -4099,20 +4147,20 @@
         <v>2</v>
       </c>
       <c r="D64" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E64" s="1" t="str">
-        <f t="shared" ref="E64:E65" si="24">TEXT(B64,"00")&amp;IF(C64="","","-"&amp;TEXT(C64,"00"))&amp;IF(D64="","","-"&amp;TEXT(D64,"00"))</f>
-        <v>06-02-05</v>
+        <f t="shared" si="22"/>
+        <v>06-02-04</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G64" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="G64" s="16" t="s">
-        <v>186</v>
-      </c>
       <c r="H64" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>23</v>
@@ -4125,7 +4173,7 @@
         <v>23</v>
       </c>
       <c r="M64" s="1" t="str">
-        <f t="shared" ref="M64:M65" si="25">IF(I64="↑","",IF(I64="-","",System_Code&amp;"_"&amp;H64&amp;IF(L64="-","","_"&amp;L64)))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="N64" s="1"/>
@@ -4143,20 +4191,20 @@
         <v>2</v>
       </c>
       <c r="D65" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1" t="str">
-        <f t="shared" si="24"/>
-        <v>06-02-06</v>
+        <f t="shared" ref="E65:E66" si="26">TEXT(B65,"00")&amp;IF(C65="","","-"&amp;TEXT(C65,"00"))&amp;IF(D65="","","-"&amp;TEXT(D65,"00"))</f>
+        <v>06-02-05</v>
       </c>
       <c r="F65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G65" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="G65" s="16" t="s">
-        <v>187</v>
-      </c>
       <c r="H65" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>23</v>
@@ -4169,7 +4217,7 @@
         <v>23</v>
       </c>
       <c r="M65" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="M65:M66" si="27">IF(I65="↑","",IF(I65="-","",System_Code&amp;"_"&amp;H65&amp;IF(L65="-","","_"&amp;L65)))</f>
         <v/>
       </c>
       <c r="N65" s="1"/>
@@ -4181,30 +4229,43 @@
         <v>62</v>
       </c>
       <c r="B66" s="1">
-        <v>7</v>
-      </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="6" t="str">
-        <f>TEXT(B66,"00")&amp;IF(C66="","","-"&amp;TEXT(C66,"00"))&amp;IF(D66="","",TEXT(D66,"00"))</f>
-        <v>07</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I66" s="7"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
-      <c r="L66" s="6"/>
-      <c r="M66" s="6"/>
-      <c r="N66" s="6"/>
-      <c r="O66" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C66" s="1">
+        <v>2</v>
+      </c>
+      <c r="D66" s="1">
+        <v>6</v>
+      </c>
+      <c r="E66" s="1" t="str">
+        <f t="shared" si="26"/>
+        <v>06-02-06</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G66" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M66" s="1" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A67" s="1">
@@ -4214,166 +4275,157 @@
       <c r="B67" s="1">
         <v>7</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="6" t="str">
+        <f>TEXT(B67,"00")&amp;IF(C67="","","-"&amp;TEXT(C67,"00"))&amp;IF(D67="","",TEXT(D67,"00"))</f>
+        <v>07</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I67" s="7"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A68" s="1">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B68" s="1">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1">
         <v>1</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1" t="str">
+      <c r="D68" s="1"/>
+      <c r="E68" s="1" t="str">
         <f t="shared" si="13"/>
         <v>07-01</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G67" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="H67" s="1" t="s">
+      <c r="F68" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I67" s="4">
-        <v>8</v>
-      </c>
-      <c r="J67" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M67" s="1" t="str">
-        <f t="shared" ref="M67:M75" si="26">IF(I67="↑","",IF(I67="-","",System_Code&amp;"_"&amp;H67&amp;IF(L67="-","","_"&amp;L67)))</f>
-        <v>SSE19_BD_SDD</v>
-      </c>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A68" s="1">
-        <f t="shared" si="3"/>
-        <v>64</v>
-      </c>
-      <c r="B68" s="1">
+      <c r="G68" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M68" s="1" t="str">
+        <f t="shared" ref="M68:M76" si="28">IF(I68="↑","",IF(I68="-","",System_Code&amp;"_"&amp;H68&amp;IF(L68="-","","_"&amp;L68)))</f>
+        <v/>
+      </c>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A69" s="1">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B69" s="1">
         <v>7</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C69" s="1">
         <v>1</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D69" s="1">
         <v>1</v>
       </c>
-      <c r="E68" s="1" t="str">
+      <c r="E69" s="1" t="str">
         <f t="shared" si="13"/>
         <v>07-01-01</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I68" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M68" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A69" s="1">
-        <f t="shared" si="3"/>
-        <v>65</v>
-      </c>
-      <c r="B69" s="1">
+      <c r="F69" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G69" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I69" s="4">
+        <v>6</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="M69" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_SDD_01_Dashboard</v>
+      </c>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A70" s="1">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="B70" s="1">
         <v>7</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C70" s="1">
         <v>1</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D70" s="1">
         <v>2</v>
       </c>
-      <c r="E69" s="1" t="str">
+      <c r="E70" s="1" t="str">
         <f t="shared" si="13"/>
         <v>07-01-02</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K69" s="1"/>
-      <c r="L69" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M69" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A70" s="1">
-        <f t="shared" si="3"/>
-        <v>66</v>
-      </c>
-      <c r="B70" s="1">
-        <v>7</v>
-      </c>
-      <c r="C70" s="1">
+      <c r="F70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G70" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I70" s="4">
         <v>2</v>
-      </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>07-02</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G70" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I70" s="4">
-        <v>8</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1" t="s">
-        <v>98</v>
+        <v>258</v>
       </c>
       <c r="M70" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v>SSE19_BD_STD</v>
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_SDD_00_Menu</v>
       </c>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -4387,21 +4439,21 @@
         <v>7</v>
       </c>
       <c r="C71" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-03</v>
+        <v>07-02</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I71" s="4">
         <v>8</v>
@@ -4409,15 +4461,13 @@
       <c r="J71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K71" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="K71" s="1"/>
       <c r="L71" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="M71" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v>SSE19_BD_RDD</v>
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_STD</v>
       </c>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
@@ -4431,21 +4481,21 @@
         <v>7</v>
       </c>
       <c r="C72" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-04</v>
+        <v>07-03</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G72" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I72" s="4">
         <v>8</v>
@@ -4453,13 +4503,15 @@
       <c r="J72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K72" s="1"/>
+      <c r="K72" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="L72" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="M72" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v>SSE19_BD_IFD</v>
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_RDD</v>
       </c>
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
@@ -4473,21 +4525,21 @@
         <v>7</v>
       </c>
       <c r="C73" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-05</v>
+        <v>07-04</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G73" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I73" s="4">
         <v>8</v>
@@ -4497,11 +4549,11 @@
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="M73" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v>SSE19_BD_API</v>
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_IFD</v>
       </c>
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
@@ -4515,21 +4567,21 @@
         <v>7</v>
       </c>
       <c r="C74" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-06</v>
+        <v>07-05</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G74" s="15" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I74" s="4">
         <v>8</v>
@@ -4539,11 +4591,11 @@
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M74" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v>SSE19_BD_BJD</v>
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_API</v>
       </c>
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
@@ -4557,35 +4609,35 @@
         <v>7</v>
       </c>
       <c r="C75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>07-07</v>
+        <v>07-06</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I75" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J75" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K75" s="1"/>
       <c r="L75" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="M75" s="1" t="str">
-        <f t="shared" si="26"/>
-        <v>SSE19_BD_FL</v>
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_BJD</v>
       </c>
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
@@ -4596,30 +4648,41 @@
         <v>72</v>
       </c>
       <c r="B76" s="1">
-        <v>8</v>
-      </c>
-      <c r="C76" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C76" s="1">
+        <v>7</v>
+      </c>
       <c r="D76" s="1"/>
-      <c r="E76" s="6" t="str">
-        <f>TEXT(B76,"00")&amp;IF(C76="","","-"&amp;TEXT(C76,"00"))&amp;IF(D76="","",TEXT(D76,"00"))</f>
-        <v>08</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I76" s="7"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
+      <c r="E76" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>07-07</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I76" s="4">
+        <v>4</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M76" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v>SSE19_BD_FL</v>
+      </c>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A77" s="1">
@@ -4629,41 +4692,28 @@
       <c r="B77" s="1">
         <v>8</v>
       </c>
-      <c r="C77" s="1">
-        <v>1</v>
-      </c>
+      <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>08-01</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G77" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H77" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I77" s="4">
-        <v>8</v>
-      </c>
-      <c r="J77" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K77" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="L77" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="M77" s="1" t="str">
-        <f>IF(I77="↑","",IF(I77="-","",System_Code&amp;"_"&amp;H77&amp;IF(L77="-","","_"&amp;L77)))</f>
-        <v>SSE19_SD_ACHS</v>
-      </c>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
+      <c r="E77" s="6" t="str">
+        <f>TEXT(B77,"00")&amp;IF(C77="","","-"&amp;TEXT(C77,"00"))&amp;IF(D77="","",TEXT(D77,"00"))</f>
+        <v>08</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G77" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I77" s="7"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+      <c r="N77" s="6"/>
+      <c r="O77" s="6"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A78" s="1">
@@ -4674,21 +4724,21 @@
         <v>8</v>
       </c>
       <c r="C78" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>08-02</v>
+        <v>08-01</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G78" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I78" s="4">
         <v>8</v>
@@ -4697,14 +4747,14 @@
         <v>13</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>124</v>
+        <v>255</v>
       </c>
       <c r="M78" s="1" t="str">
         <f>IF(I78="↑","",IF(I78="-","",System_Code&amp;"_"&amp;H78&amp;IF(L78="-","","_"&amp;L78)))</f>
-        <v>SSE19_SD_ACHA</v>
+        <v>SSE19_SD_ARCS</v>
       </c>
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
@@ -4718,37 +4768,37 @@
         <v>8</v>
       </c>
       <c r="C79" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1" t="str">
-        <f t="shared" ref="E79" si="27">TEXT(B79,"00")&amp;IF(C79="","","-"&amp;TEXT(C79,"00"))&amp;IF(D79="","","-"&amp;TEXT(D79,"00"))</f>
-        <v>08-03</v>
+        <f t="shared" si="13"/>
+        <v>08-02</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>227</v>
+        <v>119</v>
       </c>
       <c r="G79" s="15" t="s">
-        <v>228</v>
+        <v>120</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I79" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J79" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="M79" s="1" t="str">
         <f>IF(I79="↑","",IF(I79="-","",System_Code&amp;"_"&amp;H79&amp;IF(L79="-","","_"&amp;L79)))</f>
-        <v>SSE19_SD_ERD</v>
+        <v>SSE19_SD_ARCA</v>
       </c>
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
@@ -4762,71 +4812,84 @@
         <v>8</v>
       </c>
       <c r="C80" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1" t="str">
+        <f t="shared" ref="E80" si="29">TEXT(B80,"00")&amp;IF(C80="","","-"&amp;TEXT(C80,"00"))&amp;IF(D80="","","-"&amp;TEXT(D80,"00"))</f>
+        <v>08-03</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G80" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I80" s="4">
+        <v>4</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="M80" s="1" t="str">
+        <f>IF(I80="↑","",IF(I80="-","",System_Code&amp;"_"&amp;H80&amp;IF(L80="-","","_"&amp;L80)))</f>
+        <v>SSE19_SD_ERD</v>
+      </c>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A81" s="1">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="B81" s="1">
+        <v>8</v>
+      </c>
+      <c r="C81" s="1">
+        <v>4</v>
+      </c>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1" t="str">
         <f t="shared" si="13"/>
         <v>08-04</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G80" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="H80" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I80" s="4">
-        <v>4</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M80" s="1" t="str">
-        <f>IF(I80="↑","",IF(I80="-","",System_Code&amp;"_"&amp;H80&amp;IF(L80="-","","_"&amp;L80)))</f>
+      <c r="F81" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I81" s="4">
+        <v>4</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="M81" s="1" t="str">
+        <f>IF(I81="↑","",IF(I81="-","",System_Code&amp;"_"&amp;H81&amp;IF(L81="-","","_"&amp;L81)))</f>
         <v>SSE19_SD_TBLD</v>
       </c>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A81" s="1">
-        <f t="shared" si="3"/>
-        <v>77</v>
-      </c>
-      <c r="B81" s="1">
-        <v>9</v>
-      </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="6" t="str">
-        <f>TEXT(B81,"00")&amp;IF(C81="","","-"&amp;TEXT(C81,"00"))&amp;IF(D81="","",TEXT(D81,"00"))</f>
-        <v>09</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="H81" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="I81" s="7"/>
-      <c r="J81" s="6"/>
-      <c r="K81" s="6"/>
-      <c r="L81" s="6"/>
-      <c r="M81" s="6"/>
-      <c r="N81" s="6"/>
-      <c r="O81" s="6"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A82" s="1">
@@ -4836,64 +4899,53 @@
       <c r="B82" s="1">
         <v>9</v>
       </c>
-      <c r="C82" s="1">
-        <v>1</v>
-      </c>
+      <c r="C82" s="1"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="1" t="str">
-        <f t="shared" ref="E82:E83" si="28">TEXT(B82,"00")&amp;IF(C82="","","-"&amp;TEXT(C82,"00"))&amp;IF(D82="","","-"&amp;TEXT(D82,"00"))</f>
-        <v>09-01</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I82" s="4">
-        <v>4</v>
-      </c>
-      <c r="J82" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="M82" s="1" t="str">
-        <f>IF(I82="↑","",IF(I82="-","",System_Code&amp;"_"&amp;H82&amp;IF(L82="-","","_"&amp;L82)))</f>
-        <v>SSE19_Iter-pre_MVP</v>
-      </c>
-      <c r="N82" s="1"/>
-      <c r="O82" s="1"/>
+      <c r="E82" s="6" t="str">
+        <f>TEXT(B82,"00")&amp;IF(C82="","","-"&amp;TEXT(C82,"00"))&amp;IF(D82="","",TEXT(D82,"00"))</f>
+        <v>09</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="I82" s="7"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+      <c r="N82" s="6"/>
+      <c r="O82" s="6"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A83" s="1">
-        <f t="shared" ref="A83:A110" si="29">ROW()-4</f>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="B83" s="1">
         <v>9</v>
       </c>
       <c r="C83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1" t="str">
-        <f t="shared" si="28"/>
-        <v>09-02</v>
+        <f t="shared" ref="E83" si="30">TEXT(B83,"00")&amp;IF(C83="","","-"&amp;TEXT(C83,"00"))&amp;IF(D83="","","-"&amp;TEXT(D83,"00"))</f>
+        <v>09-01</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G83" s="15" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="I83" s="4">
         <v>4</v>
@@ -4903,49 +4955,60 @@
       </c>
       <c r="K83" s="1"/>
       <c r="L83" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="M83" s="1" t="str">
         <f>IF(I83="↑","",IF(I83="-","",System_Code&amp;"_"&amp;H83&amp;IF(L83="-","","_"&amp;L83)))</f>
-        <v>SSE19_Iter-pre_PBL</v>
+        <v>SSE19_Iter-pre_MVP</v>
       </c>
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A84:A112" si="31">ROW()-4</f>
         <v>80</v>
       </c>
       <c r="B84" s="1">
-        <v>10</v>
-      </c>
-      <c r="C84" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C84" s="1">
+        <v>2</v>
+      </c>
       <c r="D84" s="1"/>
-      <c r="E84" s="6" t="str">
-        <f>TEXT(B84,"00")&amp;IF(C84="","","-"&amp;TEXT(C84,"00"))&amp;IF(D84="","",TEXT(D84,"00"))</f>
-        <v>10</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G84" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H84" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="I84" s="7"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
-      <c r="L84" s="6"/>
-      <c r="M84" s="6"/>
-      <c r="N84" s="6"/>
-      <c r="O84" s="6"/>
+      <c r="E84" s="1" t="str">
+        <f t="shared" ref="E84" si="32">TEXT(B84,"00")&amp;IF(C84="","","-"&amp;TEXT(C84,"00"))&amp;IF(D84="","","-"&amp;TEXT(D84,"00"))</f>
+        <v>09-02</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G84" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="I84" s="4">
+        <v>4</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M84" s="1" t="str">
+        <f>IF(I84="↑","",IF(I84="-","",System_Code&amp;"_"&amp;H84&amp;IF(L84="-","","_"&amp;L84)))</f>
+        <v>SSE19_Iter-pre_PBL</v>
+      </c>
+      <c r="N84" s="1"/>
+      <c r="O84" s="1"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A85" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="B85" s="1">
@@ -4953,111 +5016,110 @@
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="1" t="str">
+      <c r="E85" s="6" t="str">
+        <f>TEXT(B85,"00")&amp;IF(C85="","","-"&amp;TEXT(C85,"00"))&amp;IF(D85="","",TEXT(D85,"00"))</f>
+        <v>10</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="I85" s="7"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+      <c r="O85" s="6"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A86" s="1">
+        <f t="shared" si="31"/>
+        <v>82</v>
+      </c>
+      <c r="B86" s="1">
+        <v>10</v>
+      </c>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1" t="str">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="F85" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G85" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I85" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-      <c r="M85" s="1" t="str">
-        <f>IF(I85="↑","",IF(I85="-","",System_Code&amp;"_"&amp;H85&amp;IF(L85="-","","_"&amp;L85)))</f>
-        <v/>
-      </c>
-      <c r="N85" s="1"/>
-      <c r="O85" s="1"/>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A86" s="1">
-        <f t="shared" si="29"/>
-        <v>82</v>
-      </c>
-      <c r="B86" s="1">
-        <v>10</v>
-      </c>
-      <c r="C86" s="1">
-        <v>1</v>
-      </c>
-      <c r="D86" s="1">
-        <v>1</v>
-      </c>
-      <c r="E86" s="1" t="str">
-        <f t="shared" ref="E86" si="30">TEXT(B86,"00")&amp;IF(C86="","","-"&amp;TEXT(C86,"00"))&amp;IF(D86="","","-"&amp;TEXT(D86,"00"))</f>
-        <v>10-01-01</v>
-      </c>
-      <c r="F86" s="1"/>
-      <c r="G86" s="13" t="s">
-        <v>141</v>
+      <c r="F86" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G86" s="15" t="s">
+        <v>125</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I86" s="4">
-        <v>4</v>
+        <v>233</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
+      <c r="M86" s="1" t="str">
+        <f>IF(I86="↑","",IF(I86="-","",System_Code&amp;"_"&amp;H86&amp;IF(L86="-","","_"&amp;L86)))</f>
+        <v/>
+      </c>
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
     </row>
-    <row r="87" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A87" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>83</v>
       </c>
       <c r="B87" s="1">
         <v>10</v>
       </c>
       <c r="C87" s="1">
-        <v>1</v>
-      </c>
-      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1" t="str">
+        <f>TEXT(B87,"00")&amp;IF(C87="","","-"&amp;TEXT(C87,"00"))&amp;IF(D87="","","-"&amp;TEXT(D87,"00"))</f>
+        <v>10-00</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I87" s="4">
         <v>2</v>
       </c>
-      <c r="E87" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>10-01-02</v>
-      </c>
-      <c r="F87" s="1"/>
-      <c r="G87" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="I87" s="4">
-        <v>4</v>
-      </c>
       <c r="J87" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
+      <c r="L87" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="M87" s="1" t="str">
+        <f>IF(I87="↑","",IF(I87="-","",System_Code&amp;"_"&amp;H87&amp;IF(L87="-","","_"&amp;L87)))</f>
+        <v>SSE19_Iter1_SBL</v>
+      </c>
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A88" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>84</v>
       </c>
       <c r="B88" s="1">
@@ -5067,18 +5129,18 @@
         <v>1</v>
       </c>
       <c r="D88" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E88" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>10-01-03</v>
+        <f t="shared" ref="E88" si="33">TEXT(B88,"00")&amp;IF(C88="","","-"&amp;TEXT(C88,"00"))&amp;IF(D88="","","-"&amp;TEXT(D88,"00"))</f>
+        <v>10-01-01</v>
       </c>
       <c r="F88" s="1"/>
-      <c r="G88" s="16" t="s">
-        <v>143</v>
+      <c r="G88" s="13" t="s">
+        <v>136</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I88" s="4">
         <v>4</v>
@@ -5092,9 +5154,9 @@
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A89" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>85</v>
       </c>
       <c r="B89" s="1">
@@ -5104,18 +5166,18 @@
         <v>1</v>
       </c>
       <c r="D89" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E89" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-01-04</v>
+        <v>10-01-02</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="16" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I89" s="4">
         <v>4</v>
@@ -5131,7 +5193,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A90" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>86</v>
       </c>
       <c r="B90" s="1">
@@ -5141,18 +5203,18 @@
         <v>1</v>
       </c>
       <c r="D90" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E90" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-01-05</v>
+        <v>10-01-03</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="16" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I90" s="4">
         <v>4</v>
@@ -5168,28 +5230,28 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A91" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>87</v>
       </c>
       <c r="B91" s="1">
         <v>10</v>
       </c>
       <c r="C91" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E91" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-02-01</v>
+        <v>10-01-04</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="16" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I91" s="4">
         <v>4</v>
@@ -5205,28 +5267,28 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A92" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>88</v>
       </c>
       <c r="B92" s="1">
         <v>10</v>
       </c>
       <c r="C92" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E92" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-02-02</v>
+        <v>10-01-05</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="16" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I92" s="4">
         <v>4</v>
@@ -5242,7 +5304,7 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A93" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>89</v>
       </c>
       <c r="B93" s="1">
@@ -5252,18 +5314,18 @@
         <v>2</v>
       </c>
       <c r="D93" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E93" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-02-03</v>
+        <v>10-02-01</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="16" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I93" s="4">
         <v>4</v>
@@ -5277,9 +5339,9 @@
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
     </row>
-    <row r="94" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A94" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>90</v>
       </c>
       <c r="B94" s="1">
@@ -5289,18 +5351,18 @@
         <v>2</v>
       </c>
       <c r="D94" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E94" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-02-04</v>
+        <v>10-02-02</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="16" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I94" s="4">
         <v>4</v>
@@ -5316,28 +5378,28 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A95" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>91</v>
       </c>
       <c r="B95" s="1">
         <v>10</v>
       </c>
       <c r="C95" s="1">
+        <v>2</v>
+      </c>
+      <c r="D95" s="1">
         <v>3</v>
-      </c>
-      <c r="D95" s="1">
-        <v>1</v>
       </c>
       <c r="E95" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-03-01</v>
+        <v>10-02-03</v>
       </c>
       <c r="F95" s="1"/>
-      <c r="G95" s="13" t="s">
-        <v>150</v>
+      <c r="G95" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I95" s="4">
         <v>4</v>
@@ -5353,28 +5415,28 @@
     </row>
     <row r="96" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A96" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>92</v>
       </c>
       <c r="B96" s="1">
         <v>10</v>
       </c>
       <c r="C96" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D96" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E96" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-03-02</v>
+        <v>10-02-04</v>
       </c>
       <c r="F96" s="1"/>
-      <c r="G96" s="13" t="s">
-        <v>151</v>
+      <c r="G96" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I96" s="4">
         <v>4</v>
@@ -5390,7 +5452,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A97" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>93</v>
       </c>
       <c r="B97" s="1">
@@ -5400,18 +5462,18 @@
         <v>3</v>
       </c>
       <c r="D97" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E97" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-03-03</v>
+        <v>10-03-01</v>
       </c>
       <c r="F97" s="1"/>
-      <c r="G97" s="16" t="s">
-        <v>152</v>
+      <c r="G97" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I97" s="4">
         <v>4</v>
@@ -5427,7 +5489,7 @@
     </row>
     <row r="98" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A98" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>94</v>
       </c>
       <c r="B98" s="1">
@@ -5437,18 +5499,18 @@
         <v>3</v>
       </c>
       <c r="D98" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E98" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-03-04</v>
+        <v>10-03-02</v>
       </c>
       <c r="F98" s="1"/>
-      <c r="G98" s="16" t="s">
-        <v>153</v>
+      <c r="G98" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I98" s="4">
         <v>4</v>
@@ -5462,9 +5524,9 @@
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A99" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>95</v>
       </c>
       <c r="B99" s="1">
@@ -5474,18 +5536,18 @@
         <v>3</v>
       </c>
       <c r="D99" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E99" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-03-05</v>
+        <v>10-03-03</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="16" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I99" s="4">
         <v>4</v>
@@ -5499,30 +5561,30 @@
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A100" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>96</v>
       </c>
       <c r="B100" s="1">
         <v>10</v>
       </c>
       <c r="C100" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D100" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E100" s="1" t="str">
-        <f>TEXT(B100,"00")&amp;IF(C100="","","-"&amp;TEXT(C100,"00"))&amp;IF(D100="","","-"&amp;TEXT(D100,"00"))</f>
-        <v>10-04-01</v>
+        <f t="shared" si="13"/>
+        <v>10-03-04</v>
       </c>
       <c r="F100" s="1"/>
-      <c r="G100" s="17" t="s">
-        <v>193</v>
+      <c r="G100" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I100" s="4">
         <v>4</v>
@@ -5536,30 +5598,30 @@
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A101" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>97</v>
       </c>
       <c r="B101" s="1">
         <v>10</v>
       </c>
       <c r="C101" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D101" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1" t="str">
-        <f>TEXT(B101,"00")&amp;IF(C101="","","-"&amp;TEXT(C101,"00"))&amp;IF(D101="","","-"&amp;TEXT(D101,"00"))</f>
-        <v>10-04-02</v>
+        <f t="shared" si="13"/>
+        <v>10-03-05</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="16" t="s">
-        <v>194</v>
+        <v>149</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I101" s="4">
         <v>4</v>
@@ -5575,7 +5637,7 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A102" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>98</v>
       </c>
       <c r="B102" s="1">
@@ -5585,18 +5647,18 @@
         <v>4</v>
       </c>
       <c r="D102" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E102" s="1" t="str">
         <f>TEXT(B102,"00")&amp;IF(C102="","","-"&amp;TEXT(C102,"00"))&amp;IF(D102="","","-"&amp;TEXT(D102,"00"))</f>
-        <v>10-04-03</v>
+        <v>10-04-01</v>
       </c>
       <c r="F102" s="1"/>
-      <c r="G102" s="16" t="s">
-        <v>195</v>
+      <c r="G102" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I102" s="4">
         <v>4</v>
@@ -5610,9 +5672,9 @@
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
     </row>
-    <row r="103" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A103" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>99</v>
       </c>
       <c r="B103" s="1">
@@ -5622,18 +5684,18 @@
         <v>4</v>
       </c>
       <c r="D103" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E103" s="1" t="str">
         <f>TEXT(B103,"00")&amp;IF(C103="","","-"&amp;TEXT(C103,"00"))&amp;IF(D103="","","-"&amp;TEXT(D103,"00"))</f>
-        <v>10-04-04</v>
+        <v>10-04-02</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="16" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I103" s="4">
         <v>4</v>
@@ -5649,28 +5711,28 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A104" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>100</v>
       </c>
       <c r="B104" s="1">
         <v>10</v>
       </c>
       <c r="C104" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D104" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E104" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>10-05-01</v>
+        <f>TEXT(B104,"00")&amp;IF(C104="","","-"&amp;TEXT(C104,"00"))&amp;IF(D104="","","-"&amp;TEXT(D104,"00"))</f>
+        <v>10-04-03</v>
       </c>
       <c r="F104" s="1"/>
-      <c r="G104" s="13" t="s">
-        <v>197</v>
+      <c r="G104" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I104" s="4">
         <v>4</v>
@@ -5686,28 +5748,28 @@
     </row>
     <row r="105" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A105" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>101</v>
       </c>
       <c r="B105" s="1">
         <v>10</v>
       </c>
       <c r="C105" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D105" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E105" s="1" t="str">
-        <f t="shared" si="13"/>
-        <v>10-05-02</v>
+        <f>TEXT(B105,"00")&amp;IF(C105="","","-"&amp;TEXT(C105,"00"))&amp;IF(D105="","","-"&amp;TEXT(D105,"00"))</f>
+        <v>10-04-04</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I105" s="4">
         <v>4</v>
@@ -5723,7 +5785,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A106" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>102</v>
       </c>
       <c r="B106" s="1">
@@ -5733,18 +5795,18 @@
         <v>5</v>
       </c>
       <c r="D106" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E106" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-05-03</v>
+        <v>10-05-01</v>
       </c>
       <c r="F106" s="1"/>
-      <c r="G106" s="16" t="s">
-        <v>199</v>
+      <c r="G106" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I106" s="4">
         <v>4</v>
@@ -5760,7 +5822,7 @@
     </row>
     <row r="107" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A107" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>103</v>
       </c>
       <c r="B107" s="1">
@@ -5770,18 +5832,18 @@
         <v>5</v>
       </c>
       <c r="D107" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E107" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-05-04</v>
+        <v>10-05-02</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="16" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I107" s="4">
         <v>4</v>
@@ -5795,9 +5857,9 @@
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
     </row>
-    <row r="108" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A108" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>104</v>
       </c>
       <c r="B108" s="1">
@@ -5807,18 +5869,18 @@
         <v>5</v>
       </c>
       <c r="D108" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E108" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-05-05</v>
+        <v>10-05-03</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="16" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I108" s="4">
         <v>4</v>
@@ -5834,28 +5896,28 @@
     </row>
     <row r="109" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A109" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>105</v>
       </c>
       <c r="B109" s="1">
         <v>10</v>
       </c>
       <c r="C109" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D109" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E109" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-06-01</v>
+        <v>10-05-04</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="16" t="s">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I109" s="4">
         <v>4</v>
@@ -5869,30 +5931,30 @@
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:15" ht="27" x14ac:dyDescent="0.15">
       <c r="A110" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>106</v>
       </c>
       <c r="B110" s="1">
         <v>10</v>
       </c>
       <c r="C110" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D110" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E110" s="1" t="str">
         <f t="shared" si="13"/>
-        <v>10-07-01</v>
+        <v>10-05-05</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="16" t="s">
-        <v>156</v>
+        <v>194</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="I110" s="4">
         <v>4</v>
@@ -5906,91 +5968,173 @@
       <c r="N110" s="1"/>
       <c r="O110" s="1"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="5"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="2"/>
-      <c r="N111" s="2"/>
-      <c r="O111" s="2"/>
+    <row r="111" spans="1:15" ht="27" x14ac:dyDescent="0.15">
+      <c r="A111" s="1">
+        <f t="shared" si="31"/>
+        <v>107</v>
+      </c>
+      <c r="B111" s="1">
+        <v>10</v>
+      </c>
+      <c r="C111" s="1">
+        <v>6</v>
+      </c>
+      <c r="D111" s="1">
+        <v>1</v>
+      </c>
+      <c r="E111" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-06-01</v>
+      </c>
+      <c r="F111" s="1"/>
+      <c r="G111" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I111" s="4">
+        <v>4</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K111" s="1"/>
+      <c r="L111" s="1"/>
+      <c r="M111" s="1"/>
+      <c r="N111" s="1"/>
+      <c r="O111" s="1"/>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A112" s="1">
+        <f t="shared" si="31"/>
+        <v>108</v>
+      </c>
+      <c r="B112" s="1">
+        <v>10</v>
+      </c>
+      <c r="C112" s="1">
+        <v>7</v>
+      </c>
+      <c r="D112" s="1">
+        <v>1</v>
+      </c>
+      <c r="E112" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>10-07-01</v>
+      </c>
+      <c r="F112" s="1"/>
+      <c r="G112" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I112" s="4">
+        <v>4</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K112" s="1"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="1"/>
+      <c r="O112" s="1"/>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="5"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+      <c r="N113" s="2"/>
+      <c r="O113" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:O4" xr:uid="{93992286-983A-43C0-B01F-316812382256}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="K6:K22 K29:K49 K55:K111">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+  <conditionalFormatting sqref="K6:K13 K56:K83 K29:K32 K15 K19:K22 K35:K44 K46:K50 K85:K113">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+  <conditionalFormatting sqref="K51">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="15" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="16" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K50:K51">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+  <conditionalFormatting sqref="K53:K55">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"◆済"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52:K54">
+  <conditionalFormatting sqref="K34">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"◆◆"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"◆済"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K84">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"◆◆"</formula>
     </cfRule>

</xml_diff>